<commit_message>
Update Booking Container Registration
</commit_message>
<xml_diff>
--- a/Specification/General Design Specification - Transport Management System.xlsx
+++ b/Specification/General Design Specification - Transport Management System.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/Personal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF1DCFD-3D4F-8349-AB3B-67C28FCE1CBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5F4CB4-F3C3-AF4B-97BA-466787400DC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14440" firstSheet="6" activeTab="10" xr2:uid="{E7A8EFBF-D4F9-BE40-861A-BF0B4B9B5190}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14440" firstSheet="6" activeTab="9" xr2:uid="{E7A8EFBF-D4F9-BE40-861A-BF0B4B9B5190}"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <sheet name="Draft" sheetId="10" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="249">
   <si>
     <t>No.</t>
   </si>
@@ -856,6 +855,51 @@
   </si>
   <si>
     <t>Neu ton tai ke hoach thi update, chua ton tai thi insert</t>
+  </si>
+  <si>
+    <t>Transport Schedule Inquiry</t>
+  </si>
+  <si>
+    <t>Schedule Status For Booking</t>
+  </si>
+  <si>
+    <t>full schedule</t>
+  </si>
+  <si>
+    <t>(partial schedule/empty schedule/blank)</t>
+  </si>
+  <si>
+    <t>ETD from</t>
+  </si>
+  <si>
+    <t>ETD To</t>
+  </si>
+  <si>
+    <t>ETA from</t>
+  </si>
+  <si>
+    <t>ETA To</t>
+  </si>
+  <si>
+    <t>Container truck</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>Search empty schedule la liet ke cac booking chua co schedule. Cot action la schedule. Khi click vao schedule thi qua man hinh Transport Schedule Registration va show o tab for booking</t>
+  </si>
+  <si>
+    <t>Search partial liet ke tat ca cac booking da co schedule mot phan. Cot action la edit. Khi click vao schedule thi qua man hinh Transport Schedule Registration va show o tab for booking</t>
+  </si>
+  <si>
+    <t>Note: Search full schedule liet ke tat ca cac booking da co schedule. Cot action la edit. Khi click vao schedule thi qua man hinh Transport Schedule Registration va show o tab for booking</t>
+  </si>
+  <si>
+    <t>Note: tong so luong booking la 2 + 3 la 5 thi tuong ung co 5 dong du lieu de nhap lieu va save</t>
+  </si>
+  <si>
+    <t>Khi click vao search button thi show thong tin mau xam tu thong tin booking da tao.</t>
   </si>
 </sst>
 </file>
@@ -1398,7 +1442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1494,6 +1538,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1650,7 +1696,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5578,6 +5673,137 @@
 
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E154149F-5EF1-D147-8250-289EC5297FE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4445000" y="838200"/>
+          <a:ext cx="622300" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Search</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A4C3210-546E-0342-B18E-1C150F166634}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8255000" y="2260600"/>
+          <a:ext cx="622300" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Search</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -6032,10 +6258,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E1F607D-F349-1E4C-A80B-CC18273F07C4}">
-  <dimension ref="B2:AM24"/>
+  <dimension ref="B2:AM29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AE27" sqref="AE27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="AP19" sqref="AP19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
@@ -6188,62 +6414,63 @@
     </row>
     <row r="8" spans="2:39">
       <c r="C8" s="8"/>
-      <c r="D8" s="119" t="s">
+      <c r="D8" s="145" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="120"/>
-      <c r="F8" s="119" t="s">
+      <c r="E8" s="146"/>
+      <c r="F8" s="145" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="120"/>
-      <c r="H8" s="119" t="s">
+      <c r="G8" s="146"/>
+      <c r="H8" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="129"/>
-      <c r="J8" s="129"/>
-      <c r="K8" s="129"/>
-      <c r="L8" s="129"/>
-      <c r="M8" s="120"/>
-      <c r="N8" s="119" t="s">
+      <c r="I8" s="147"/>
+      <c r="J8" s="147"/>
+      <c r="K8" s="147"/>
+      <c r="L8" s="147"/>
+      <c r="M8" s="146"/>
+      <c r="N8" s="145" t="s">
         <v>72</v>
       </c>
-      <c r="O8" s="129"/>
-      <c r="P8" s="120"/>
+      <c r="O8" s="147"/>
+      <c r="P8" s="146"/>
       <c r="Q8" s="9"/>
-      <c r="R8" s="9" t="s">
+      <c r="R8" s="161" t="s">
         <v>144</v>
       </c>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9" t="s">
+      <c r="S8" s="161"/>
+      <c r="T8" s="161" t="s">
         <v>145</v>
       </c>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
+      <c r="U8" s="161"/>
+      <c r="V8" s="161"/>
+      <c r="W8" s="161"/>
+      <c r="X8" s="161"/>
+      <c r="Y8" s="161"/>
+      <c r="Z8" s="161"/>
+      <c r="AA8" s="161"/>
+      <c r="AB8" s="161"/>
+      <c r="AC8" s="161"/>
+      <c r="AD8" s="161"/>
+      <c r="AE8" s="162"/>
       <c r="AG8" s="10"/>
     </row>
     <row r="9" spans="2:39">
       <c r="C9" s="8"/>
-      <c r="D9" s="121"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="121"/>
-      <c r="G9" s="122"/>
-      <c r="H9" s="121"/>
-      <c r="I9" s="130"/>
-      <c r="J9" s="130"/>
-      <c r="K9" s="130"/>
-      <c r="L9" s="130"/>
-      <c r="M9" s="122"/>
-      <c r="N9" s="121"/>
-      <c r="O9" s="130"/>
-      <c r="P9" s="122"/>
+      <c r="D9" s="148"/>
+      <c r="E9" s="149"/>
+      <c r="F9" s="148"/>
+      <c r="G9" s="149"/>
+      <c r="H9" s="148"/>
+      <c r="I9" s="150"/>
+      <c r="J9" s="150"/>
+      <c r="K9" s="150"/>
+      <c r="L9" s="150"/>
+      <c r="M9" s="149"/>
+      <c r="N9" s="148"/>
+      <c r="O9" s="150"/>
+      <c r="P9" s="149"/>
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
@@ -6262,27 +6489,27 @@
     </row>
     <row r="10" spans="2:39">
       <c r="C10" s="8"/>
-      <c r="D10" s="119" t="s">
+      <c r="D10" s="145" t="s">
         <v>142</v>
       </c>
-      <c r="E10" s="120"/>
-      <c r="F10" s="132">
+      <c r="E10" s="146"/>
+      <c r="F10" s="151">
         <v>2</v>
       </c>
-      <c r="G10" s="133"/>
-      <c r="H10" s="123">
+      <c r="G10" s="152"/>
+      <c r="H10" s="153">
         <v>0</v>
       </c>
-      <c r="I10" s="127"/>
-      <c r="J10" s="127"/>
-      <c r="K10" s="127"/>
-      <c r="L10" s="127"/>
-      <c r="M10" s="124"/>
-      <c r="N10" s="123">
+      <c r="I10" s="154"/>
+      <c r="J10" s="154"/>
+      <c r="K10" s="154"/>
+      <c r="L10" s="154"/>
+      <c r="M10" s="155"/>
+      <c r="N10" s="153">
         <v>0</v>
       </c>
-      <c r="O10" s="127"/>
-      <c r="P10" s="124"/>
+      <c r="O10" s="154"/>
+      <c r="P10" s="155"/>
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
@@ -6301,19 +6528,19 @@
     </row>
     <row r="11" spans="2:39">
       <c r="C11" s="8"/>
-      <c r="D11" s="121"/>
-      <c r="E11" s="122"/>
-      <c r="F11" s="134"/>
-      <c r="G11" s="135"/>
-      <c r="H11" s="125"/>
-      <c r="I11" s="128"/>
-      <c r="J11" s="128"/>
-      <c r="K11" s="128"/>
-      <c r="L11" s="128"/>
-      <c r="M11" s="126"/>
-      <c r="N11" s="125"/>
-      <c r="O11" s="128"/>
-      <c r="P11" s="126"/>
+      <c r="D11" s="148"/>
+      <c r="E11" s="149"/>
+      <c r="F11" s="156"/>
+      <c r="G11" s="157"/>
+      <c r="H11" s="158"/>
+      <c r="I11" s="159"/>
+      <c r="J11" s="159"/>
+      <c r="K11" s="159"/>
+      <c r="L11" s="159"/>
+      <c r="M11" s="160"/>
+      <c r="N11" s="158"/>
+      <c r="O11" s="159"/>
+      <c r="P11" s="160"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
@@ -6332,27 +6559,27 @@
     </row>
     <row r="12" spans="2:39">
       <c r="C12" s="8"/>
-      <c r="D12" s="119" t="s">
+      <c r="D12" s="145" t="s">
         <v>143</v>
       </c>
-      <c r="E12" s="120"/>
-      <c r="F12" s="132">
+      <c r="E12" s="146"/>
+      <c r="F12" s="151">
         <v>3</v>
       </c>
-      <c r="G12" s="133"/>
-      <c r="H12" s="123">
+      <c r="G12" s="152"/>
+      <c r="H12" s="153">
         <v>0</v>
       </c>
-      <c r="I12" s="127"/>
-      <c r="J12" s="127"/>
-      <c r="K12" s="127"/>
-      <c r="L12" s="127"/>
-      <c r="M12" s="124"/>
-      <c r="N12" s="123">
+      <c r="I12" s="154"/>
+      <c r="J12" s="154"/>
+      <c r="K12" s="154"/>
+      <c r="L12" s="154"/>
+      <c r="M12" s="155"/>
+      <c r="N12" s="153">
         <v>0</v>
       </c>
-      <c r="O12" s="127"/>
-      <c r="P12" s="124"/>
+      <c r="O12" s="154"/>
+      <c r="P12" s="155"/>
       <c r="Q12" s="9"/>
       <c r="R12" s="9"/>
       <c r="S12" s="9"/>
@@ -6371,19 +6598,19 @@
     </row>
     <row r="13" spans="2:39">
       <c r="C13" s="8"/>
-      <c r="D13" s="121"/>
-      <c r="E13" s="122"/>
-      <c r="F13" s="134"/>
-      <c r="G13" s="135"/>
-      <c r="H13" s="125"/>
-      <c r="I13" s="128"/>
-      <c r="J13" s="128"/>
-      <c r="K13" s="128"/>
-      <c r="L13" s="128"/>
-      <c r="M13" s="126"/>
-      <c r="N13" s="125"/>
-      <c r="O13" s="128"/>
-      <c r="P13" s="126"/>
+      <c r="D13" s="148"/>
+      <c r="E13" s="149"/>
+      <c r="F13" s="156"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="158"/>
+      <c r="I13" s="159"/>
+      <c r="J13" s="159"/>
+      <c r="K13" s="159"/>
+      <c r="L13" s="159"/>
+      <c r="M13" s="160"/>
+      <c r="N13" s="158"/>
+      <c r="O13" s="159"/>
+      <c r="P13" s="160"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="9"/>
       <c r="S13" s="9"/>
@@ -6555,32 +6782,32 @@
       <c r="S17" s="30">
         <v>1</v>
       </c>
-      <c r="T17" s="136">
+      <c r="T17" s="138">
         <v>10</v>
       </c>
-      <c r="U17" s="137"/>
-      <c r="V17" s="136">
+      <c r="U17" s="139"/>
+      <c r="V17" s="138">
         <v>5</v>
       </c>
-      <c r="W17" s="137"/>
+      <c r="W17" s="139"/>
       <c r="X17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Y17" s="136">
+      <c r="Y17" s="138">
         <v>0</v>
       </c>
-      <c r="Z17" s="138"/>
-      <c r="AA17" s="137"/>
-      <c r="AB17" s="139"/>
-      <c r="AC17" s="140"/>
-      <c r="AD17" s="139"/>
-      <c r="AE17" s="140"/>
-      <c r="AF17" s="139" t="s">
+      <c r="Z17" s="140"/>
+      <c r="AA17" s="139"/>
+      <c r="AB17" s="141"/>
+      <c r="AC17" s="142"/>
+      <c r="AD17" s="141"/>
+      <c r="AE17" s="142"/>
+      <c r="AF17" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="AG17" s="141"/>
-      <c r="AL17" s="142"/>
-      <c r="AM17" s="142"/>
+      <c r="AG17" s="143"/>
+      <c r="AL17" s="144"/>
+      <c r="AM17" s="144"/>
     </row>
     <row r="18" spans="3:39">
       <c r="C18" s="8"/>
@@ -6612,32 +6839,32 @@
       <c r="S18" s="30">
         <v>1</v>
       </c>
-      <c r="T18" s="136">
+      <c r="T18" s="138">
         <v>11</v>
       </c>
-      <c r="U18" s="137"/>
-      <c r="V18" s="136">
+      <c r="U18" s="139"/>
+      <c r="V18" s="138">
         <v>6</v>
       </c>
-      <c r="W18" s="137"/>
+      <c r="W18" s="139"/>
       <c r="X18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Y18" s="136">
+      <c r="Y18" s="138">
         <v>1</v>
       </c>
-      <c r="Z18" s="138"/>
-      <c r="AA18" s="137"/>
-      <c r="AB18" s="139"/>
-      <c r="AC18" s="140"/>
-      <c r="AD18" s="139"/>
-      <c r="AE18" s="140"/>
-      <c r="AF18" s="139" t="s">
+      <c r="Z18" s="140"/>
+      <c r="AA18" s="139"/>
+      <c r="AB18" s="141"/>
+      <c r="AC18" s="142"/>
+      <c r="AD18" s="141"/>
+      <c r="AE18" s="142"/>
+      <c r="AF18" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="AG18" s="141"/>
-      <c r="AL18" s="142"/>
-      <c r="AM18" s="142"/>
+      <c r="AG18" s="143"/>
+      <c r="AL18" s="144"/>
+      <c r="AM18" s="144"/>
     </row>
     <row r="19" spans="3:39">
       <c r="C19" s="8"/>
@@ -6669,32 +6896,32 @@
       <c r="S19" s="30">
         <v>1</v>
       </c>
-      <c r="T19" s="136">
+      <c r="T19" s="138">
         <v>12</v>
       </c>
-      <c r="U19" s="137"/>
-      <c r="V19" s="136">
+      <c r="U19" s="139"/>
+      <c r="V19" s="138">
         <v>7</v>
       </c>
-      <c r="W19" s="137"/>
+      <c r="W19" s="139"/>
       <c r="X19" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Y19" s="136">
+      <c r="Y19" s="138">
         <v>2</v>
       </c>
-      <c r="Z19" s="138"/>
-      <c r="AA19" s="137"/>
-      <c r="AB19" s="139"/>
-      <c r="AC19" s="140"/>
-      <c r="AD19" s="139"/>
-      <c r="AE19" s="140"/>
-      <c r="AF19" s="139" t="s">
+      <c r="Z19" s="140"/>
+      <c r="AA19" s="139"/>
+      <c r="AB19" s="141"/>
+      <c r="AC19" s="142"/>
+      <c r="AD19" s="141"/>
+      <c r="AE19" s="142"/>
+      <c r="AF19" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="AG19" s="141"/>
-      <c r="AL19" s="142"/>
-      <c r="AM19" s="142"/>
+      <c r="AG19" s="143"/>
+      <c r="AL19" s="144"/>
+      <c r="AM19" s="144"/>
     </row>
     <row r="20" spans="3:39">
       <c r="C20" s="8"/>
@@ -6726,32 +6953,32 @@
       <c r="S20" s="30">
         <v>1</v>
       </c>
-      <c r="T20" s="136">
+      <c r="T20" s="138">
         <v>13</v>
       </c>
-      <c r="U20" s="137"/>
-      <c r="V20" s="136">
+      <c r="U20" s="139"/>
+      <c r="V20" s="138">
         <v>8</v>
       </c>
-      <c r="W20" s="137"/>
+      <c r="W20" s="139"/>
       <c r="X20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Y20" s="136">
+      <c r="Y20" s="138">
         <v>3</v>
       </c>
-      <c r="Z20" s="138"/>
-      <c r="AA20" s="137"/>
-      <c r="AB20" s="139"/>
-      <c r="AC20" s="140"/>
-      <c r="AD20" s="139"/>
-      <c r="AE20" s="140"/>
-      <c r="AF20" s="139" t="s">
+      <c r="Z20" s="140"/>
+      <c r="AA20" s="139"/>
+      <c r="AB20" s="141"/>
+      <c r="AC20" s="142"/>
+      <c r="AD20" s="141"/>
+      <c r="AE20" s="142"/>
+      <c r="AF20" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="AG20" s="141"/>
-      <c r="AL20" s="142"/>
-      <c r="AM20" s="142"/>
+      <c r="AG20" s="143"/>
+      <c r="AL20" s="144"/>
+      <c r="AM20" s="144"/>
     </row>
     <row r="21" spans="3:39">
       <c r="C21" s="8"/>
@@ -6783,32 +7010,32 @@
       <c r="S21" s="30">
         <v>1</v>
       </c>
-      <c r="T21" s="136">
+      <c r="T21" s="138">
         <v>14</v>
       </c>
-      <c r="U21" s="137"/>
-      <c r="V21" s="136">
+      <c r="U21" s="139"/>
+      <c r="V21" s="138">
         <v>9</v>
       </c>
-      <c r="W21" s="137"/>
+      <c r="W21" s="139"/>
       <c r="X21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Y21" s="136">
+      <c r="Y21" s="138">
         <v>4</v>
       </c>
-      <c r="Z21" s="138"/>
-      <c r="AA21" s="137"/>
-      <c r="AB21" s="139"/>
-      <c r="AC21" s="140"/>
-      <c r="AD21" s="139"/>
-      <c r="AE21" s="140"/>
-      <c r="AF21" s="139" t="s">
+      <c r="Z21" s="140"/>
+      <c r="AA21" s="139"/>
+      <c r="AB21" s="141"/>
+      <c r="AC21" s="142"/>
+      <c r="AD21" s="141"/>
+      <c r="AE21" s="142"/>
+      <c r="AF21" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="AG21" s="141"/>
-      <c r="AL21" s="142"/>
-      <c r="AM21" s="142"/>
+      <c r="AG21" s="143"/>
+      <c r="AL21" s="144"/>
+      <c r="AM21" s="144"/>
     </row>
     <row r="22" spans="3:39">
       <c r="C22" s="8"/>
@@ -6911,6 +7138,70 @@
       <c r="AE24" s="12"/>
       <c r="AF24" s="12"/>
       <c r="AG24" s="13"/>
+    </row>
+    <row r="27" spans="3:39">
+      <c r="D27" s="91" t="s">
+        <v>247</v>
+      </c>
+      <c r="E27" s="91"/>
+      <c r="F27" s="91"/>
+      <c r="G27" s="91"/>
+      <c r="H27" s="91"/>
+      <c r="I27" s="91"/>
+      <c r="J27" s="91"/>
+      <c r="K27" s="91"/>
+      <c r="L27" s="91"/>
+      <c r="M27" s="91"/>
+      <c r="N27" s="91"/>
+      <c r="O27" s="91"/>
+      <c r="P27" s="91"/>
+      <c r="Q27" s="91"/>
+      <c r="R27" s="91"/>
+      <c r="S27" s="91"/>
+      <c r="T27" s="91"/>
+      <c r="U27" s="91"/>
+    </row>
+    <row r="28" spans="3:39">
+      <c r="D28" s="91"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="91"/>
+      <c r="H28" s="91"/>
+      <c r="I28" s="91"/>
+      <c r="J28" s="91"/>
+      <c r="K28" s="91"/>
+      <c r="L28" s="91"/>
+      <c r="M28" s="91"/>
+      <c r="N28" s="91"/>
+      <c r="O28" s="91"/>
+      <c r="P28" s="91"/>
+      <c r="Q28" s="91"/>
+      <c r="R28" s="91"/>
+      <c r="S28" s="91"/>
+      <c r="T28" s="91"/>
+      <c r="U28" s="91"/>
+    </row>
+    <row r="29" spans="3:39">
+      <c r="D29" s="91"/>
+      <c r="E29" s="91" t="s">
+        <v>248</v>
+      </c>
+      <c r="F29" s="91"/>
+      <c r="G29" s="91"/>
+      <c r="H29" s="91"/>
+      <c r="I29" s="91"/>
+      <c r="J29" s="91"/>
+      <c r="K29" s="91"/>
+      <c r="L29" s="91"/>
+      <c r="M29" s="91"/>
+      <c r="N29" s="91"/>
+      <c r="O29" s="91"/>
+      <c r="P29" s="91"/>
+      <c r="Q29" s="91"/>
+      <c r="R29" s="91"/>
+      <c r="S29" s="91"/>
+      <c r="T29" s="91"/>
+      <c r="U29" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="47">
@@ -6971,8 +7262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{074DFE09-608C-C946-A127-D7CE93149F2F}">
   <dimension ref="C2:AV76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:AQ18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
@@ -10250,12 +10541,12 @@
       <c r="AV68" s="13"/>
     </row>
     <row r="72" spans="3:48">
-      <c r="D72" s="143" t="s">
+      <c r="D72" s="91" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="74" spans="3:48">
-      <c r="E74" s="143" t="s">
+      <c r="E74" s="91" t="s">
         <v>232</v>
       </c>
     </row>
@@ -10272,15 +10563,1736 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD9D15D-AD2D-D04C-8C57-C9E8723A1ED0}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:AV33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="AR27" sqref="AR27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="2:48" ht="17" thickBot="1"/>
+    <row r="2" spans="2:48" ht="17" thickBot="1">
+      <c r="B2" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
+      <c r="AF2" s="25"/>
+      <c r="AG2" s="25"/>
+      <c r="AH2" s="25"/>
+      <c r="AI2" s="25"/>
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
+      <c r="AO2" s="25"/>
+      <c r="AP2" s="25"/>
+      <c r="AQ2" s="25"/>
+      <c r="AR2" s="25"/>
+      <c r="AS2" s="25"/>
+      <c r="AT2" s="25"/>
+      <c r="AU2" s="25"/>
+      <c r="AV2" s="26"/>
+    </row>
+    <row r="3" spans="2:48">
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="92" t="s">
+        <v>237</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="9"/>
+      <c r="AK3" s="9"/>
+      <c r="AL3" s="9"/>
+      <c r="AM3" s="9"/>
+      <c r="AN3" s="9"/>
+      <c r="AO3" s="9"/>
+      <c r="AP3" s="9"/>
+      <c r="AQ3" s="9"/>
+      <c r="AR3" s="9"/>
+      <c r="AS3" s="9"/>
+      <c r="AT3" s="9"/>
+      <c r="AU3" s="9"/>
+      <c r="AV3" s="10"/>
+    </row>
+    <row r="4" spans="2:48">
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="9"/>
+      <c r="AN4" s="9"/>
+      <c r="AO4" s="9"/>
+      <c r="AP4" s="9"/>
+      <c r="AQ4" s="9"/>
+      <c r="AR4" s="9"/>
+      <c r="AS4" s="9"/>
+      <c r="AT4" s="9"/>
+      <c r="AU4" s="9"/>
+      <c r="AV4" s="10"/>
+    </row>
+    <row r="5" spans="2:48">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="9"/>
+      <c r="AK5" s="9"/>
+      <c r="AL5" s="9"/>
+      <c r="AM5" s="9"/>
+      <c r="AN5" s="9"/>
+      <c r="AO5" s="9"/>
+      <c r="AP5" s="9"/>
+      <c r="AQ5" s="9"/>
+      <c r="AR5" s="9"/>
+      <c r="AS5" s="9"/>
+      <c r="AT5" s="9"/>
+      <c r="AU5" s="9"/>
+      <c r="AV5" s="10"/>
+    </row>
+    <row r="6" spans="2:48">
+      <c r="B6" s="68"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="69"/>
+      <c r="Q6" s="69"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="69"/>
+      <c r="T6" s="69"/>
+      <c r="U6" s="69"/>
+      <c r="V6" s="69"/>
+      <c r="W6" s="69"/>
+      <c r="X6" s="69"/>
+      <c r="Y6" s="69"/>
+      <c r="Z6" s="69"/>
+      <c r="AA6" s="69"/>
+      <c r="AB6" s="69"/>
+      <c r="AC6" s="69"/>
+      <c r="AD6" s="69"/>
+      <c r="AE6" s="69"/>
+      <c r="AF6" s="69"/>
+      <c r="AG6" s="69"/>
+      <c r="AH6" s="69"/>
+      <c r="AI6" s="69"/>
+      <c r="AJ6" s="69"/>
+      <c r="AK6" s="69"/>
+      <c r="AL6" s="69"/>
+      <c r="AM6" s="69"/>
+      <c r="AN6" s="69"/>
+      <c r="AO6" s="69"/>
+      <c r="AP6" s="69"/>
+      <c r="AQ6" s="69"/>
+      <c r="AR6" s="69"/>
+      <c r="AS6" s="69"/>
+      <c r="AT6" s="69"/>
+      <c r="AU6" s="69"/>
+      <c r="AV6" s="70"/>
+    </row>
+    <row r="7" spans="2:48">
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9"/>
+      <c r="AQ7" s="9"/>
+      <c r="AR7" s="9"/>
+      <c r="AS7" s="9"/>
+      <c r="AT7" s="9"/>
+      <c r="AU7" s="9"/>
+      <c r="AV7" s="10"/>
+    </row>
+    <row r="8" spans="2:48">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="29"/>
+      <c r="Y8" s="30"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="9"/>
+      <c r="AN8" s="9"/>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="9"/>
+      <c r="AQ8" s="9"/>
+      <c r="AR8" s="9"/>
+      <c r="AS8" s="9"/>
+      <c r="AT8" s="9"/>
+      <c r="AU8" s="9"/>
+      <c r="AV8" s="10"/>
+    </row>
+    <row r="9" spans="2:48">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+      <c r="AP9" s="9"/>
+      <c r="AQ9" s="9"/>
+      <c r="AR9" s="9"/>
+      <c r="AS9" s="9"/>
+      <c r="AT9" s="9"/>
+      <c r="AU9" s="9"/>
+      <c r="AV9" s="10"/>
+    </row>
+    <row r="10" spans="2:48">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="K10" s="9"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="9"/>
+      <c r="AO10" s="9"/>
+      <c r="AP10" s="9"/>
+      <c r="AQ10" s="9"/>
+      <c r="AR10" s="9"/>
+      <c r="AS10" s="9"/>
+      <c r="AT10" s="9"/>
+      <c r="AU10" s="9"/>
+      <c r="AV10" s="10"/>
+    </row>
+    <row r="11" spans="2:48">
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
+      <c r="AP11" s="9"/>
+      <c r="AQ11" s="9"/>
+      <c r="AR11" s="9"/>
+      <c r="AS11" s="9"/>
+      <c r="AT11" s="9"/>
+      <c r="AU11" s="9"/>
+      <c r="AV11" s="10"/>
+    </row>
+    <row r="12" spans="2:48">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="K12" s="9"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
+      <c r="AN12" s="9"/>
+      <c r="AO12" s="9"/>
+      <c r="AP12" s="9"/>
+      <c r="AQ12" s="9"/>
+      <c r="AR12" s="9"/>
+      <c r="AS12" s="9"/>
+      <c r="AT12" s="9"/>
+      <c r="AU12" s="9"/>
+      <c r="AV12" s="10"/>
+    </row>
+    <row r="13" spans="2:48">
+      <c r="B13" s="68"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="69"/>
+      <c r="N13" s="69"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="69"/>
+      <c r="Q13" s="69"/>
+      <c r="R13" s="69"/>
+      <c r="S13" s="69"/>
+      <c r="T13" s="69"/>
+      <c r="U13" s="69"/>
+      <c r="V13" s="69"/>
+      <c r="W13" s="69"/>
+      <c r="X13" s="69"/>
+      <c r="Y13" s="69"/>
+      <c r="Z13" s="69"/>
+      <c r="AA13" s="69"/>
+      <c r="AB13" s="69"/>
+      <c r="AC13" s="69"/>
+      <c r="AD13" s="69"/>
+      <c r="AE13" s="69"/>
+      <c r="AF13" s="69"/>
+      <c r="AG13" s="69"/>
+      <c r="AH13" s="69"/>
+      <c r="AI13" s="69"/>
+      <c r="AJ13" s="69"/>
+      <c r="AK13" s="69"/>
+      <c r="AL13" s="69"/>
+      <c r="AM13" s="69"/>
+      <c r="AN13" s="69"/>
+      <c r="AO13" s="69"/>
+      <c r="AP13" s="69"/>
+      <c r="AQ13" s="69"/>
+      <c r="AR13" s="69"/>
+      <c r="AS13" s="69"/>
+      <c r="AT13" s="69"/>
+      <c r="AU13" s="69"/>
+      <c r="AV13" s="70"/>
+    </row>
+    <row r="14" spans="2:48">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="9"/>
+      <c r="AI14" s="9"/>
+      <c r="AJ14" s="9"/>
+      <c r="AK14" s="9"/>
+      <c r="AL14" s="28">
+        <v>20</v>
+      </c>
+      <c r="AM14" s="29"/>
+      <c r="AN14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO14" s="9"/>
+      <c r="AP14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ14" s="2">
+        <v>2</v>
+      </c>
+      <c r="AR14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AS14" s="2">
+        <v>3</v>
+      </c>
+      <c r="AT14" s="2">
+        <v>4</v>
+      </c>
+      <c r="AU14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AV14" s="10"/>
+    </row>
+    <row r="15" spans="2:48" ht="17" thickBot="1">
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="9"/>
+      <c r="AJ15" s="9"/>
+      <c r="AK15" s="9"/>
+      <c r="AL15" s="9"/>
+      <c r="AM15" s="9"/>
+      <c r="AN15" s="9"/>
+      <c r="AO15" s="9"/>
+      <c r="AP15" s="9"/>
+      <c r="AQ15" s="9"/>
+      <c r="AR15" s="9"/>
+      <c r="AS15" s="9"/>
+      <c r="AT15" s="9"/>
+      <c r="AU15" s="9"/>
+      <c r="AV15" s="10"/>
+    </row>
+    <row r="16" spans="2:48">
+      <c r="B16" s="8"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="6"/>
+      <c r="AI16" s="6"/>
+      <c r="AJ16" s="6"/>
+      <c r="AK16" s="6"/>
+      <c r="AL16" s="6"/>
+      <c r="AM16" s="6"/>
+      <c r="AN16" s="6"/>
+      <c r="AO16" s="6"/>
+      <c r="AP16" s="6"/>
+      <c r="AQ16" s="6"/>
+      <c r="AR16" s="6"/>
+      <c r="AS16" s="6"/>
+      <c r="AT16" s="6"/>
+      <c r="AU16" s="7"/>
+      <c r="AV16" s="10"/>
+    </row>
+    <row r="17" spans="2:48">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="71" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="72"/>
+      <c r="F17" s="71" t="s">
+        <v>189</v>
+      </c>
+      <c r="G17" s="73"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="J17" s="73"/>
+      <c r="K17" s="71" t="s">
+        <v>197</v>
+      </c>
+      <c r="L17" s="72"/>
+      <c r="M17" s="71" t="s">
+        <v>144</v>
+      </c>
+      <c r="N17" s="73"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="72"/>
+      <c r="Q17" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="16"/>
+      <c r="Z17" s="16"/>
+      <c r="AA17" s="16"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="AD17" s="16"/>
+      <c r="AE17" s="16"/>
+      <c r="AF17" s="17"/>
+      <c r="AG17" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="AH17" s="16"/>
+      <c r="AI17" s="17"/>
+      <c r="AJ17" s="71" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK17" s="73"/>
+      <c r="AL17" s="73"/>
+      <c r="AM17" s="73"/>
+      <c r="AN17" s="72"/>
+      <c r="AO17" s="16"/>
+      <c r="AP17" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="AQ17" s="17"/>
+      <c r="AR17" s="9"/>
+      <c r="AS17" s="9"/>
+      <c r="AT17" s="9"/>
+      <c r="AU17" s="10"/>
+      <c r="AV17" s="10"/>
+    </row>
+    <row r="18" spans="2:48">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="74"/>
+      <c r="L18" s="75"/>
+      <c r="M18" s="74"/>
+      <c r="N18" s="76"/>
+      <c r="O18" s="76"/>
+      <c r="P18" s="75"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="21"/>
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="21"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="20"/>
+      <c r="AD18" s="21"/>
+      <c r="AE18" s="21"/>
+      <c r="AF18" s="22"/>
+      <c r="AG18" s="20"/>
+      <c r="AH18" s="21"/>
+      <c r="AI18" s="22"/>
+      <c r="AJ18" s="74"/>
+      <c r="AK18" s="76"/>
+      <c r="AL18" s="76"/>
+      <c r="AM18" s="76"/>
+      <c r="AN18" s="75"/>
+      <c r="AO18" s="21"/>
+      <c r="AP18" s="21"/>
+      <c r="AQ18" s="22"/>
+      <c r="AR18" s="9"/>
+      <c r="AS18" s="9"/>
+      <c r="AT18" s="9"/>
+      <c r="AU18" s="10"/>
+      <c r="AV18" s="10"/>
+    </row>
+    <row r="19" spans="2:48">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="71">
+        <v>1</v>
+      </c>
+      <c r="E19" s="72"/>
+      <c r="F19" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="G19" s="73"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="71" t="s">
+        <v>142</v>
+      </c>
+      <c r="J19" s="73"/>
+      <c r="K19" s="71" t="s">
+        <v>209</v>
+      </c>
+      <c r="L19" s="72"/>
+      <c r="M19" s="71" t="s">
+        <v>210</v>
+      </c>
+      <c r="N19" s="73"/>
+      <c r="O19" s="73"/>
+      <c r="P19" s="72"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="Y19" s="16"/>
+      <c r="Z19" s="16"/>
+      <c r="AA19" s="16"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD19" s="16"/>
+      <c r="AE19" s="16"/>
+      <c r="AF19" s="17"/>
+      <c r="AG19" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="AH19" s="16"/>
+      <c r="AI19" s="17"/>
+      <c r="AJ19" s="71" t="s">
+        <v>207</v>
+      </c>
+      <c r="AK19" s="73"/>
+      <c r="AL19" s="73"/>
+      <c r="AM19" s="73"/>
+      <c r="AN19" s="72"/>
+      <c r="AO19" s="16"/>
+      <c r="AP19" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="AQ19" s="17"/>
+      <c r="AR19" s="9"/>
+      <c r="AS19" s="92"/>
+      <c r="AT19" s="9"/>
+      <c r="AU19" s="10"/>
+      <c r="AV19" s="10"/>
+    </row>
+    <row r="20" spans="2:48">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="74"/>
+      <c r="N20" s="76"/>
+      <c r="O20" s="76"/>
+      <c r="P20" s="75"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="22"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="21"/>
+      <c r="Z20" s="21"/>
+      <c r="AA20" s="21"/>
+      <c r="AB20" s="22"/>
+      <c r="AC20" s="20"/>
+      <c r="AD20" s="21"/>
+      <c r="AE20" s="21"/>
+      <c r="AF20" s="22"/>
+      <c r="AG20" s="20"/>
+      <c r="AH20" s="21"/>
+      <c r="AI20" s="22"/>
+      <c r="AJ20" s="74"/>
+      <c r="AK20" s="76"/>
+      <c r="AL20" s="76"/>
+      <c r="AM20" s="76"/>
+      <c r="AN20" s="75"/>
+      <c r="AO20" s="21"/>
+      <c r="AP20" s="21"/>
+      <c r="AQ20" s="22"/>
+      <c r="AR20" s="9"/>
+      <c r="AS20" s="9"/>
+      <c r="AT20" s="9"/>
+      <c r="AU20" s="10"/>
+      <c r="AV20" s="10"/>
+    </row>
+    <row r="21" spans="2:48">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="71">
+        <v>2</v>
+      </c>
+      <c r="E21" s="72"/>
+      <c r="F21" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="G21" s="73"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="71" t="s">
+        <v>142</v>
+      </c>
+      <c r="J21" s="73"/>
+      <c r="K21" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="L21" s="72"/>
+      <c r="M21" s="71" t="s">
+        <v>210</v>
+      </c>
+      <c r="N21" s="73"/>
+      <c r="O21" s="73"/>
+      <c r="P21" s="72"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="Y21" s="16"/>
+      <c r="Z21" s="16"/>
+      <c r="AA21" s="16"/>
+      <c r="AB21" s="17"/>
+      <c r="AC21" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="AD21" s="16"/>
+      <c r="AE21" s="16"/>
+      <c r="AF21" s="17"/>
+      <c r="AG21" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH21" s="16"/>
+      <c r="AI21" s="17"/>
+      <c r="AJ21" s="71" t="s">
+        <v>207</v>
+      </c>
+      <c r="AK21" s="73"/>
+      <c r="AL21" s="73"/>
+      <c r="AM21" s="73"/>
+      <c r="AN21" s="72"/>
+      <c r="AO21" s="16"/>
+      <c r="AP21" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="AQ21" s="17"/>
+      <c r="AR21" s="9"/>
+      <c r="AS21" s="9"/>
+      <c r="AT21" s="9"/>
+      <c r="AU21" s="10"/>
+      <c r="AV21" s="10"/>
+    </row>
+    <row r="22" spans="2:48">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="75"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="76"/>
+      <c r="O22" s="76"/>
+      <c r="P22" s="75"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="22"/>
+      <c r="W22" s="20"/>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="21"/>
+      <c r="Z22" s="21"/>
+      <c r="AA22" s="21"/>
+      <c r="AB22" s="22"/>
+      <c r="AC22" s="20"/>
+      <c r="AD22" s="21"/>
+      <c r="AE22" s="21"/>
+      <c r="AF22" s="22"/>
+      <c r="AG22" s="20"/>
+      <c r="AH22" s="21"/>
+      <c r="AI22" s="22"/>
+      <c r="AJ22" s="74"/>
+      <c r="AK22" s="76"/>
+      <c r="AL22" s="76"/>
+      <c r="AM22" s="76"/>
+      <c r="AN22" s="75"/>
+      <c r="AO22" s="21"/>
+      <c r="AP22" s="21"/>
+      <c r="AQ22" s="22"/>
+      <c r="AR22" s="9"/>
+      <c r="AS22" s="9"/>
+      <c r="AT22" s="9"/>
+      <c r="AU22" s="10"/>
+      <c r="AV22" s="10"/>
+    </row>
+    <row r="23" spans="2:48">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="71">
+        <v>3</v>
+      </c>
+      <c r="E23" s="72"/>
+      <c r="F23" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="G23" s="73"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="71" t="s">
+        <v>142</v>
+      </c>
+      <c r="J23" s="73"/>
+      <c r="K23" s="71" t="s">
+        <v>227</v>
+      </c>
+      <c r="L23" s="72"/>
+      <c r="M23" s="71" t="s">
+        <v>210</v>
+      </c>
+      <c r="N23" s="73"/>
+      <c r="O23" s="73"/>
+      <c r="P23" s="72"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="16"/>
+      <c r="AB23" s="17"/>
+      <c r="AC23" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD23" s="16"/>
+      <c r="AE23" s="16"/>
+      <c r="AF23" s="17"/>
+      <c r="AG23" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="AH23" s="16"/>
+      <c r="AI23" s="17"/>
+      <c r="AJ23" s="71" t="s">
+        <v>207</v>
+      </c>
+      <c r="AK23" s="73"/>
+      <c r="AL23" s="73"/>
+      <c r="AM23" s="73"/>
+      <c r="AN23" s="72"/>
+      <c r="AO23" s="16"/>
+      <c r="AP23" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="AQ23" s="17"/>
+      <c r="AR23" s="9"/>
+      <c r="AS23" s="9"/>
+      <c r="AT23" s="9"/>
+      <c r="AU23" s="10"/>
+      <c r="AV23" s="10"/>
+    </row>
+    <row r="24" spans="2:48">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="74"/>
+      <c r="L24" s="75"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="76"/>
+      <c r="O24" s="76"/>
+      <c r="P24" s="75"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="22"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="21"/>
+      <c r="Y24" s="21"/>
+      <c r="Z24" s="21"/>
+      <c r="AA24" s="21"/>
+      <c r="AB24" s="22"/>
+      <c r="AC24" s="20"/>
+      <c r="AD24" s="21"/>
+      <c r="AE24" s="21"/>
+      <c r="AF24" s="22"/>
+      <c r="AG24" s="20"/>
+      <c r="AH24" s="21"/>
+      <c r="AI24" s="22"/>
+      <c r="AJ24" s="74"/>
+      <c r="AK24" s="76"/>
+      <c r="AL24" s="76"/>
+      <c r="AM24" s="76"/>
+      <c r="AN24" s="75"/>
+      <c r="AO24" s="21"/>
+      <c r="AP24" s="21"/>
+      <c r="AQ24" s="22"/>
+      <c r="AR24" s="9"/>
+      <c r="AS24" s="9"/>
+      <c r="AT24" s="9"/>
+      <c r="AU24" s="10"/>
+      <c r="AV24" s="10"/>
+    </row>
+    <row r="25" spans="2:48">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="9"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9"/>
+      <c r="AF25" s="9"/>
+      <c r="AG25" s="9"/>
+      <c r="AH25" s="9"/>
+      <c r="AI25" s="9"/>
+      <c r="AJ25" s="9"/>
+      <c r="AK25" s="9"/>
+      <c r="AL25" s="9"/>
+      <c r="AM25" s="9"/>
+      <c r="AN25" s="9"/>
+      <c r="AO25" s="9"/>
+      <c r="AP25" s="9"/>
+      <c r="AQ25" s="9"/>
+      <c r="AR25" s="9"/>
+      <c r="AS25" s="9"/>
+      <c r="AT25" s="9"/>
+      <c r="AU25" s="10"/>
+      <c r="AV25" s="10"/>
+    </row>
+    <row r="26" spans="2:48">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="92" t="s">
+        <v>246</v>
+      </c>
+      <c r="F26" s="92"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="92"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="92"/>
+      <c r="K26" s="92"/>
+      <c r="L26" s="92"/>
+      <c r="M26" s="92"/>
+      <c r="N26" s="92"/>
+      <c r="O26" s="92"/>
+      <c r="P26" s="92"/>
+      <c r="Q26" s="92"/>
+      <c r="R26" s="92"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="9"/>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
+      <c r="AF26" s="9"/>
+      <c r="AG26" s="9"/>
+      <c r="AH26" s="9"/>
+      <c r="AI26" s="9"/>
+      <c r="AJ26" s="9"/>
+      <c r="AK26" s="9"/>
+      <c r="AL26" s="9"/>
+      <c r="AM26" s="9"/>
+      <c r="AN26" s="9"/>
+      <c r="AO26" s="9"/>
+      <c r="AP26" s="9"/>
+      <c r="AQ26" s="9"/>
+      <c r="AR26" s="9"/>
+      <c r="AS26" s="9"/>
+      <c r="AT26" s="9"/>
+      <c r="AU26" s="10"/>
+      <c r="AV26" s="10"/>
+    </row>
+    <row r="27" spans="2:48">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="92"/>
+      <c r="F27" s="92" t="s">
+        <v>245</v>
+      </c>
+      <c r="G27" s="92"/>
+      <c r="H27" s="92"/>
+      <c r="I27" s="92"/>
+      <c r="J27" s="92"/>
+      <c r="K27" s="92"/>
+      <c r="L27" s="92"/>
+      <c r="M27" s="92"/>
+      <c r="N27" s="92"/>
+      <c r="O27" s="92"/>
+      <c r="P27" s="92"/>
+      <c r="Q27" s="92"/>
+      <c r="R27" s="92"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AB27" s="9"/>
+      <c r="AC27" s="9"/>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="9"/>
+      <c r="AG27" s="9"/>
+      <c r="AH27" s="9"/>
+      <c r="AI27" s="9"/>
+      <c r="AJ27" s="9"/>
+      <c r="AK27" s="9"/>
+      <c r="AL27" s="9"/>
+      <c r="AM27" s="9"/>
+      <c r="AN27" s="9"/>
+      <c r="AO27" s="9"/>
+      <c r="AP27" s="9"/>
+      <c r="AQ27" s="9"/>
+      <c r="AR27" s="9"/>
+      <c r="AS27" s="9"/>
+      <c r="AT27" s="9"/>
+      <c r="AU27" s="10"/>
+      <c r="AV27" s="10"/>
+    </row>
+    <row r="28" spans="2:48">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="92" t="s">
+        <v>244</v>
+      </c>
+      <c r="G28" s="92"/>
+      <c r="H28" s="92"/>
+      <c r="I28" s="92"/>
+      <c r="J28" s="92"/>
+      <c r="K28" s="92"/>
+      <c r="L28" s="92"/>
+      <c r="M28" s="92"/>
+      <c r="N28" s="92"/>
+      <c r="O28" s="92"/>
+      <c r="P28" s="92"/>
+      <c r="Q28" s="92"/>
+      <c r="R28" s="92"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+      <c r="AA28" s="9"/>
+      <c r="AB28" s="9"/>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="9"/>
+      <c r="AF28" s="9"/>
+      <c r="AG28" s="9"/>
+      <c r="AH28" s="9"/>
+      <c r="AI28" s="9"/>
+      <c r="AJ28" s="9"/>
+      <c r="AK28" s="9"/>
+      <c r="AL28" s="9"/>
+      <c r="AM28" s="9"/>
+      <c r="AN28" s="9"/>
+      <c r="AO28" s="9"/>
+      <c r="AP28" s="9"/>
+      <c r="AQ28" s="9"/>
+      <c r="AR28" s="9"/>
+      <c r="AS28" s="9"/>
+      <c r="AT28" s="9"/>
+      <c r="AU28" s="10"/>
+      <c r="AV28" s="10"/>
+    </row>
+    <row r="29" spans="2:48">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="9"/>
+      <c r="Z29" s="9"/>
+      <c r="AA29" s="9"/>
+      <c r="AB29" s="9"/>
+      <c r="AC29" s="9"/>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="9"/>
+      <c r="AF29" s="9"/>
+      <c r="AG29" s="9"/>
+      <c r="AH29" s="9"/>
+      <c r="AI29" s="9"/>
+      <c r="AJ29" s="9"/>
+      <c r="AK29" s="9"/>
+      <c r="AL29" s="9"/>
+      <c r="AM29" s="9"/>
+      <c r="AN29" s="9"/>
+      <c r="AO29" s="9"/>
+      <c r="AP29" s="9"/>
+      <c r="AQ29" s="9"/>
+      <c r="AR29" s="9"/>
+      <c r="AS29" s="9"/>
+      <c r="AT29" s="9"/>
+      <c r="AU29" s="10"/>
+      <c r="AV29" s="10"/>
+    </row>
+    <row r="30" spans="2:48" ht="17" thickBot="1">
+      <c r="B30" s="8"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="12"/>
+      <c r="AA30" s="12"/>
+      <c r="AB30" s="12"/>
+      <c r="AC30" s="12"/>
+      <c r="AD30" s="12"/>
+      <c r="AE30" s="12"/>
+      <c r="AF30" s="12"/>
+      <c r="AG30" s="12"/>
+      <c r="AH30" s="12"/>
+      <c r="AI30" s="12"/>
+      <c r="AJ30" s="12"/>
+      <c r="AK30" s="12"/>
+      <c r="AL30" s="12"/>
+      <c r="AM30" s="12"/>
+      <c r="AN30" s="12"/>
+      <c r="AO30" s="12"/>
+      <c r="AP30" s="12"/>
+      <c r="AQ30" s="12"/>
+      <c r="AR30" s="12"/>
+      <c r="AS30" s="12"/>
+      <c r="AT30" s="12"/>
+      <c r="AU30" s="13"/>
+      <c r="AV30" s="10"/>
+    </row>
+    <row r="31" spans="2:48">
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
+      <c r="AB31" s="9"/>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="9"/>
+      <c r="AG31" s="9"/>
+      <c r="AH31" s="9"/>
+      <c r="AI31" s="9"/>
+      <c r="AJ31" s="9"/>
+      <c r="AK31" s="9"/>
+      <c r="AL31" s="9"/>
+      <c r="AM31" s="9"/>
+      <c r="AN31" s="9"/>
+      <c r="AO31" s="9"/>
+      <c r="AP31" s="9"/>
+      <c r="AQ31" s="9"/>
+      <c r="AR31" s="9"/>
+      <c r="AS31" s="9"/>
+      <c r="AT31" s="9"/>
+      <c r="AU31" s="9"/>
+      <c r="AV31" s="10"/>
+    </row>
+    <row r="32" spans="2:48">
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
+      <c r="W32" s="9"/>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="9"/>
+      <c r="Z32" s="9"/>
+      <c r="AA32" s="9"/>
+      <c r="AB32" s="9"/>
+      <c r="AC32" s="9"/>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="9"/>
+      <c r="AF32" s="9"/>
+      <c r="AG32" s="9"/>
+      <c r="AH32" s="9"/>
+      <c r="AI32" s="9"/>
+      <c r="AJ32" s="9"/>
+      <c r="AK32" s="9"/>
+      <c r="AL32" s="28">
+        <v>20</v>
+      </c>
+      <c r="AM32" s="29"/>
+      <c r="AN32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO32" s="9"/>
+      <c r="AP32" s="2">
+        <v>1</v>
+      </c>
+      <c r="AQ32" s="2">
+        <v>2</v>
+      </c>
+      <c r="AR32" s="2">
+        <v>3</v>
+      </c>
+      <c r="AS32" s="2">
+        <v>3</v>
+      </c>
+      <c r="AT32" s="2">
+        <v>4</v>
+      </c>
+      <c r="AU32" s="2">
+        <v>5</v>
+      </c>
+      <c r="AV32" s="10"/>
+    </row>
+    <row r="33" spans="2:48" ht="17" thickBot="1">
+      <c r="B33" s="11"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="12"/>
+      <c r="W33" s="12"/>
+      <c r="X33" s="12"/>
+      <c r="Y33" s="12"/>
+      <c r="Z33" s="12"/>
+      <c r="AA33" s="12"/>
+      <c r="AB33" s="12"/>
+      <c r="AC33" s="12"/>
+      <c r="AD33" s="12"/>
+      <c r="AE33" s="12"/>
+      <c r="AF33" s="12"/>
+      <c r="AG33" s="12"/>
+      <c r="AH33" s="12"/>
+      <c r="AI33" s="12"/>
+      <c r="AJ33" s="12"/>
+      <c r="AK33" s="12"/>
+      <c r="AL33" s="12"/>
+      <c r="AM33" s="12"/>
+      <c r="AN33" s="12"/>
+      <c r="AO33" s="12"/>
+      <c r="AP33" s="12"/>
+      <c r="AQ33" s="12"/>
+      <c r="AR33" s="12"/>
+      <c r="AS33" s="12"/>
+      <c r="AT33" s="12"/>
+      <c r="AU33" s="12"/>
+      <c r="AV33" s="13"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10549,15 +12561,15 @@
     </row>
     <row r="3" spans="2:36" ht="17" thickBot="1"/>
     <row r="4" spans="2:36">
-      <c r="F4" s="103" t="s">
+      <c r="F4" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="104"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="105"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="107"/>
       <c r="M4" s="5"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -10569,28 +12581,28 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
-      <c r="X4" s="109" t="s">
+      <c r="X4" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="Y4" s="110"/>
-      <c r="Z4" s="110"/>
-      <c r="AA4" s="110"/>
-      <c r="AB4" s="110"/>
-      <c r="AC4" s="110"/>
-      <c r="AD4" s="110"/>
-      <c r="AE4" s="110"/>
-      <c r="AF4" s="110"/>
-      <c r="AG4" s="110"/>
-      <c r="AH4" s="111"/>
+      <c r="Y4" s="112"/>
+      <c r="Z4" s="112"/>
+      <c r="AA4" s="112"/>
+      <c r="AB4" s="112"/>
+      <c r="AC4" s="112"/>
+      <c r="AD4" s="112"/>
+      <c r="AE4" s="112"/>
+      <c r="AF4" s="112"/>
+      <c r="AG4" s="112"/>
+      <c r="AH4" s="113"/>
     </row>
     <row r="5" spans="2:36" ht="17" thickBot="1">
-      <c r="F5" s="106"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="110"/>
       <c r="M5" s="11"/>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
@@ -10602,31 +12614,31 @@
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
-      <c r="X5" s="112"/>
-      <c r="Y5" s="113"/>
-      <c r="Z5" s="113"/>
-      <c r="AA5" s="113"/>
-      <c r="AB5" s="113"/>
-      <c r="AC5" s="113"/>
-      <c r="AD5" s="113"/>
-      <c r="AE5" s="113"/>
-      <c r="AF5" s="113"/>
-      <c r="AG5" s="113"/>
-      <c r="AH5" s="114"/>
+      <c r="X5" s="114"/>
+      <c r="Y5" s="115"/>
+      <c r="Z5" s="115"/>
+      <c r="AA5" s="115"/>
+      <c r="AB5" s="115"/>
+      <c r="AC5" s="115"/>
+      <c r="AD5" s="115"/>
+      <c r="AE5" s="115"/>
+      <c r="AF5" s="115"/>
+      <c r="AG5" s="115"/>
+      <c r="AH5" s="116"/>
       <c r="AJ5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:36">
-      <c r="F6" s="97" t="s">
+      <c r="F6" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="99"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="101"/>
       <c r="M6" s="5"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -10651,13 +12663,13 @@
       <c r="AH6" s="7"/>
     </row>
     <row r="7" spans="2:36" ht="17" thickBot="1">
-      <c r="F7" s="100"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="104"/>
       <c r="M7" s="8"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -10682,15 +12694,15 @@
       <c r="AH7" s="10"/>
     </row>
     <row r="8" spans="2:36">
-      <c r="F8" s="91" t="s">
+      <c r="F8" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="93"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="95"/>
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -10717,13 +12729,13 @@
       <c r="AH8" s="10"/>
     </row>
     <row r="9" spans="2:36" ht="17" thickBot="1">
-      <c r="F9" s="94"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="95"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="95"/>
-      <c r="K9" s="95"/>
-      <c r="L9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="98"/>
       <c r="M9" s="8"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -10748,15 +12760,15 @@
       <c r="AH9" s="10"/>
     </row>
     <row r="10" spans="2:36">
-      <c r="F10" s="91" t="s">
+      <c r="F10" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="93"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="94"/>
+      <c r="I10" s="94"/>
+      <c r="J10" s="94"/>
+      <c r="K10" s="94"/>
+      <c r="L10" s="95"/>
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -10781,13 +12793,13 @@
       <c r="AH10" s="10"/>
     </row>
     <row r="11" spans="2:36" ht="17" thickBot="1">
-      <c r="F11" s="94"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="95"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="97"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="98"/>
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -10812,15 +12824,15 @@
       <c r="AH11" s="10"/>
     </row>
     <row r="12" spans="2:36" ht="16" customHeight="1">
-      <c r="F12" s="91" t="s">
+      <c r="F12" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="93"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="94"/>
+      <c r="I12" s="94"/>
+      <c r="J12" s="94"/>
+      <c r="K12" s="94"/>
+      <c r="L12" s="95"/>
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -10845,13 +12857,13 @@
       <c r="AH12" s="10"/>
     </row>
     <row r="13" spans="2:36" ht="17" thickBot="1">
-      <c r="F13" s="94"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="95"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="95"/>
-      <c r="K13" s="95"/>
-      <c r="L13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="98"/>
       <c r="M13" s="11"/>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
@@ -10876,15 +12888,15 @@
       <c r="AH13" s="13"/>
     </row>
     <row r="14" spans="2:36" ht="16" customHeight="1">
-      <c r="F14" s="91" t="s">
+      <c r="F14" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="93"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="94"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="95"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
@@ -10909,13 +12921,13 @@
       <c r="AH14" s="10"/>
     </row>
     <row r="15" spans="2:36" ht="17" thickBot="1">
-      <c r="F15" s="94"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="95"/>
-      <c r="L15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="97"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="98"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
@@ -10940,15 +12952,15 @@
       <c r="AH15" s="10"/>
     </row>
     <row r="16" spans="2:36">
-      <c r="F16" s="91" t="s">
+      <c r="F16" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="93"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="95"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
@@ -10973,13 +12985,13 @@
       <c r="AH16" s="10"/>
     </row>
     <row r="17" spans="2:36" ht="17" thickBot="1">
-      <c r="F17" s="94"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="97"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="98"/>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
@@ -11004,15 +13016,15 @@
       <c r="AH17" s="10"/>
     </row>
     <row r="18" spans="2:36" ht="16" customHeight="1">
-      <c r="F18" s="91" t="s">
+      <c r="F18" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
-      <c r="K18" s="92"/>
-      <c r="L18" s="93"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="95"/>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
@@ -11037,13 +13049,13 @@
       <c r="AH18" s="10"/>
     </row>
     <row r="19" spans="2:36" ht="17" thickBot="1">
-      <c r="F19" s="94"/>
-      <c r="G19" s="95"/>
-      <c r="H19" s="95"/>
-      <c r="I19" s="95"/>
-      <c r="J19" s="95"/>
-      <c r="K19" s="95"/>
-      <c r="L19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="97"/>
+      <c r="K19" s="97"/>
+      <c r="L19" s="98"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
@@ -11068,15 +13080,15 @@
       <c r="AH19" s="10"/>
     </row>
     <row r="20" spans="2:36">
-      <c r="F20" s="91" t="s">
+      <c r="F20" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="92"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="92"/>
-      <c r="K20" s="92"/>
-      <c r="L20" s="93"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="94"/>
+      <c r="J20" s="94"/>
+      <c r="K20" s="94"/>
+      <c r="L20" s="95"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
@@ -11101,13 +13113,13 @@
       <c r="AH20" s="10"/>
     </row>
     <row r="21" spans="2:36" ht="17" thickBot="1">
-      <c r="F21" s="94"/>
-      <c r="G21" s="95"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="95"/>
-      <c r="J21" s="95"/>
-      <c r="K21" s="95"/>
-      <c r="L21" s="96"/>
+      <c r="F21" s="96"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="97"/>
+      <c r="I21" s="97"/>
+      <c r="J21" s="97"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="98"/>
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
@@ -11572,15 +13584,15 @@
     </row>
     <row r="3" spans="2:73" ht="17" thickBot="1"/>
     <row r="4" spans="2:73" ht="17" thickBot="1">
-      <c r="F4" s="103" t="s">
+      <c r="F4" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="104"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="105"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="107"/>
       <c r="M4" s="5"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -11592,19 +13604,19 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
-      <c r="X4" s="109" t="s">
+      <c r="X4" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="Y4" s="110"/>
-      <c r="Z4" s="110"/>
-      <c r="AA4" s="110"/>
-      <c r="AB4" s="110"/>
-      <c r="AC4" s="110"/>
-      <c r="AD4" s="110"/>
-      <c r="AE4" s="110"/>
-      <c r="AF4" s="110"/>
-      <c r="AG4" s="110"/>
-      <c r="AH4" s="111"/>
+      <c r="Y4" s="112"/>
+      <c r="Z4" s="112"/>
+      <c r="AA4" s="112"/>
+      <c r="AB4" s="112"/>
+      <c r="AC4" s="112"/>
+      <c r="AD4" s="112"/>
+      <c r="AE4" s="112"/>
+      <c r="AF4" s="112"/>
+      <c r="AG4" s="112"/>
+      <c r="AH4" s="113"/>
       <c r="AR4" s="24" t="s">
         <v>14</v>
       </c>
@@ -11639,13 +13651,13 @@
       <c r="BU4" s="26"/>
     </row>
     <row r="5" spans="2:73" ht="17" thickBot="1">
-      <c r="F5" s="106"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="110"/>
       <c r="M5" s="11"/>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
@@ -11657,17 +13669,17 @@
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
-      <c r="X5" s="112"/>
-      <c r="Y5" s="113"/>
-      <c r="Z5" s="113"/>
-      <c r="AA5" s="113"/>
-      <c r="AB5" s="113"/>
-      <c r="AC5" s="113"/>
-      <c r="AD5" s="113"/>
-      <c r="AE5" s="113"/>
-      <c r="AF5" s="113"/>
-      <c r="AG5" s="113"/>
-      <c r="AH5" s="114"/>
+      <c r="X5" s="114"/>
+      <c r="Y5" s="115"/>
+      <c r="Z5" s="115"/>
+      <c r="AA5" s="115"/>
+      <c r="AB5" s="115"/>
+      <c r="AC5" s="115"/>
+      <c r="AD5" s="115"/>
+      <c r="AE5" s="115"/>
+      <c r="AF5" s="115"/>
+      <c r="AG5" s="115"/>
+      <c r="AH5" s="116"/>
       <c r="AJ5" t="s">
         <v>36</v>
       </c>
@@ -11703,15 +13715,15 @@
       <c r="BU5" s="10"/>
     </row>
     <row r="6" spans="2:73">
-      <c r="F6" s="97" t="s">
+      <c r="F6" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="99"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="101"/>
       <c r="M6" s="5"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -11766,13 +13778,13 @@
       <c r="BU6" s="10"/>
     </row>
     <row r="7" spans="2:73" ht="17" thickBot="1">
-      <c r="F7" s="100"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="104"/>
       <c r="M7" s="8"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -11827,15 +13839,15 @@
       <c r="BU7" s="10"/>
     </row>
     <row r="8" spans="2:73">
-      <c r="F8" s="91" t="s">
+      <c r="F8" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="93"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="95"/>
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -11890,13 +13902,13 @@
       <c r="BU8" s="10"/>
     </row>
     <row r="9" spans="2:73" ht="17" thickBot="1">
-      <c r="F9" s="94"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="95"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="95"/>
-      <c r="K9" s="95"/>
-      <c r="L9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="98"/>
       <c r="M9" s="8"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -11951,15 +13963,15 @@
       <c r="BU9" s="10"/>
     </row>
     <row r="10" spans="2:73">
-      <c r="F10" s="91" t="s">
+      <c r="F10" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="93"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="94"/>
+      <c r="I10" s="94"/>
+      <c r="J10" s="94"/>
+      <c r="K10" s="94"/>
+      <c r="L10" s="95"/>
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -12014,13 +14026,13 @@
       <c r="BU10" s="10"/>
     </row>
     <row r="11" spans="2:73" ht="17" thickBot="1">
-      <c r="F11" s="94"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="95"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="97"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="98"/>
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -12075,15 +14087,15 @@
       <c r="BU11" s="10"/>
     </row>
     <row r="12" spans="2:73" ht="16" customHeight="1">
-      <c r="F12" s="91" t="s">
+      <c r="F12" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="93"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="94"/>
+      <c r="I12" s="94"/>
+      <c r="J12" s="94"/>
+      <c r="K12" s="94"/>
+      <c r="L12" s="95"/>
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -12138,13 +14150,13 @@
       <c r="BU12" s="10"/>
     </row>
     <row r="13" spans="2:73" ht="17" thickBot="1">
-      <c r="F13" s="94"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="95"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="95"/>
-      <c r="K13" s="95"/>
-      <c r="L13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="98"/>
       <c r="M13" s="11"/>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
@@ -12199,15 +14211,15 @@
       <c r="BU13" s="10"/>
     </row>
     <row r="14" spans="2:73" ht="16" customHeight="1">
-      <c r="F14" s="91" t="s">
+      <c r="F14" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="93"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="94"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="95"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
@@ -12262,13 +14274,13 @@
       <c r="BU14" s="10"/>
     </row>
     <row r="15" spans="2:73" ht="17" thickBot="1">
-      <c r="F15" s="94"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="95"/>
-      <c r="L15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="97"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="98"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
@@ -12323,15 +14335,15 @@
       <c r="BU15" s="10"/>
     </row>
     <row r="16" spans="2:73">
-      <c r="F16" s="91" t="s">
+      <c r="F16" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="93"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="95"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
@@ -12386,13 +14398,13 @@
       <c r="BU16" s="10"/>
     </row>
     <row r="17" spans="2:73" ht="17" thickBot="1">
-      <c r="F17" s="94"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="97"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="98"/>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
@@ -12447,15 +14459,15 @@
       <c r="BU17" s="10"/>
     </row>
     <row r="18" spans="2:73" ht="16" customHeight="1">
-      <c r="F18" s="91" t="s">
+      <c r="F18" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
-      <c r="K18" s="92"/>
-      <c r="L18" s="93"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="95"/>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
@@ -12510,13 +14522,13 @@
       <c r="BU18" s="10"/>
     </row>
     <row r="19" spans="2:73" ht="17" thickBot="1">
-      <c r="F19" s="94"/>
-      <c r="G19" s="95"/>
-      <c r="H19" s="95"/>
-      <c r="I19" s="95"/>
-      <c r="J19" s="95"/>
-      <c r="K19" s="95"/>
-      <c r="L19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="97"/>
+      <c r="K19" s="97"/>
+      <c r="L19" s="98"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
@@ -12571,15 +14583,15 @@
       <c r="BU19" s="10"/>
     </row>
     <row r="20" spans="2:73">
-      <c r="F20" s="91" t="s">
+      <c r="F20" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="92"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="92"/>
-      <c r="K20" s="92"/>
-      <c r="L20" s="93"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="94"/>
+      <c r="J20" s="94"/>
+      <c r="K20" s="94"/>
+      <c r="L20" s="95"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
@@ -12634,13 +14646,13 @@
       <c r="BU20" s="10"/>
     </row>
     <row r="21" spans="2:73" ht="17" thickBot="1">
-      <c r="F21" s="94"/>
-      <c r="G21" s="95"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="95"/>
-      <c r="J21" s="95"/>
-      <c r="K21" s="95"/>
-      <c r="L21" s="96"/>
+      <c r="F21" s="96"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="97"/>
+      <c r="I21" s="97"/>
+      <c r="J21" s="97"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="98"/>
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
@@ -13024,15 +15036,15 @@
     </row>
     <row r="3" spans="2:164" ht="17" thickBot="1"/>
     <row r="4" spans="2:164" ht="17" thickBot="1">
-      <c r="F4" s="103" t="s">
+      <c r="F4" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="104"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="105"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="107"/>
       <c r="M4" s="5"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -13044,19 +15056,19 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
-      <c r="X4" s="109" t="s">
+      <c r="X4" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="Y4" s="110"/>
-      <c r="Z4" s="110"/>
-      <c r="AA4" s="110"/>
-      <c r="AB4" s="110"/>
-      <c r="AC4" s="110"/>
-      <c r="AD4" s="110"/>
-      <c r="AE4" s="110"/>
-      <c r="AF4" s="110"/>
-      <c r="AG4" s="110"/>
-      <c r="AH4" s="111"/>
+      <c r="Y4" s="112"/>
+      <c r="Z4" s="112"/>
+      <c r="AA4" s="112"/>
+      <c r="AB4" s="112"/>
+      <c r="AC4" s="112"/>
+      <c r="AD4" s="112"/>
+      <c r="AE4" s="112"/>
+      <c r="AF4" s="112"/>
+      <c r="AG4" s="112"/>
+      <c r="AH4" s="113"/>
       <c r="AR4" s="24" t="s">
         <v>18</v>
       </c>
@@ -13182,13 +15194,13 @@
       <c r="FH4" s="26"/>
     </row>
     <row r="5" spans="2:164" ht="17" thickBot="1">
-      <c r="F5" s="106"/>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="110"/>
       <c r="M5" s="11"/>
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
@@ -13200,17 +15212,17 @@
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
-      <c r="X5" s="112"/>
-      <c r="Y5" s="113"/>
-      <c r="Z5" s="113"/>
-      <c r="AA5" s="113"/>
-      <c r="AB5" s="113"/>
-      <c r="AC5" s="113"/>
-      <c r="AD5" s="113"/>
-      <c r="AE5" s="113"/>
-      <c r="AF5" s="113"/>
-      <c r="AG5" s="113"/>
-      <c r="AH5" s="114"/>
+      <c r="X5" s="114"/>
+      <c r="Y5" s="115"/>
+      <c r="Z5" s="115"/>
+      <c r="AA5" s="115"/>
+      <c r="AB5" s="115"/>
+      <c r="AC5" s="115"/>
+      <c r="AD5" s="115"/>
+      <c r="AE5" s="115"/>
+      <c r="AF5" s="115"/>
+      <c r="AG5" s="115"/>
+      <c r="AH5" s="116"/>
       <c r="AJ5" t="s">
         <v>36</v>
       </c>
@@ -13347,15 +15359,15 @@
       <c r="FH5" s="10"/>
     </row>
     <row r="6" spans="2:164">
-      <c r="F6" s="97" t="s">
+      <c r="F6" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="99"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="100"/>
+      <c r="I6" s="100"/>
+      <c r="J6" s="100"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="101"/>
       <c r="M6" s="5"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -13497,13 +15509,13 @@
       <c r="FH6" s="10"/>
     </row>
     <row r="7" spans="2:164" ht="17" customHeight="1" thickBot="1">
-      <c r="F7" s="100"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="103"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="103"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="104"/>
       <c r="M7" s="8"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
@@ -13666,15 +15678,15 @@
       <c r="FH7" s="10"/>
     </row>
     <row r="8" spans="2:164">
-      <c r="F8" s="91" t="s">
+      <c r="F8" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="93"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="95"/>
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
@@ -13783,27 +15795,27 @@
       <c r="DY8" s="19"/>
       <c r="DZ8" s="10"/>
       <c r="EC8" s="8"/>
-      <c r="ED8" s="119" t="s">
+      <c r="ED8" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="EE8" s="120"/>
-      <c r="EF8" s="119" t="s">
+      <c r="EE8" s="122"/>
+      <c r="EF8" s="121" t="s">
         <v>70</v>
       </c>
-      <c r="EG8" s="120"/>
-      <c r="EH8" s="119" t="s">
+      <c r="EG8" s="122"/>
+      <c r="EH8" s="121" t="s">
         <v>71</v>
       </c>
-      <c r="EI8" s="129"/>
-      <c r="EJ8" s="129"/>
-      <c r="EK8" s="129"/>
-      <c r="EL8" s="129"/>
-      <c r="EM8" s="120"/>
-      <c r="EN8" s="119" t="s">
+      <c r="EI8" s="131"/>
+      <c r="EJ8" s="131"/>
+      <c r="EK8" s="131"/>
+      <c r="EL8" s="131"/>
+      <c r="EM8" s="122"/>
+      <c r="EN8" s="121" t="s">
         <v>72</v>
       </c>
-      <c r="EO8" s="129"/>
-      <c r="EP8" s="120"/>
+      <c r="EO8" s="131"/>
+      <c r="EP8" s="122"/>
       <c r="EQ8" s="9"/>
       <c r="ER8" s="9" t="s">
         <v>144</v>
@@ -13827,13 +15839,13 @@
       <c r="FH8" s="10"/>
     </row>
     <row r="9" spans="2:164" ht="17" thickBot="1">
-      <c r="F9" s="94"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="95"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="95"/>
-      <c r="K9" s="95"/>
-      <c r="L9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="98"/>
       <c r="M9" s="8"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
@@ -13933,11 +15945,11 @@
       <c r="DJ9" s="9"/>
       <c r="DK9" s="19"/>
       <c r="DL9" s="9"/>
-      <c r="DM9" s="117" t="s">
+      <c r="DM9" s="119" t="s">
         <v>112</v>
       </c>
-      <c r="DN9" s="118"/>
-      <c r="DO9" s="118"/>
+      <c r="DN9" s="120"/>
+      <c r="DO9" s="120"/>
       <c r="DP9" s="15"/>
       <c r="DQ9" s="16"/>
       <c r="DR9" s="16"/>
@@ -13950,19 +15962,19 @@
       <c r="DY9" s="17"/>
       <c r="DZ9" s="10"/>
       <c r="EC9" s="8"/>
-      <c r="ED9" s="121"/>
-      <c r="EE9" s="122"/>
-      <c r="EF9" s="121"/>
-      <c r="EG9" s="122"/>
-      <c r="EH9" s="121"/>
-      <c r="EI9" s="130"/>
-      <c r="EJ9" s="130"/>
-      <c r="EK9" s="130"/>
-      <c r="EL9" s="130"/>
-      <c r="EM9" s="122"/>
-      <c r="EN9" s="121"/>
-      <c r="EO9" s="130"/>
-      <c r="EP9" s="122"/>
+      <c r="ED9" s="123"/>
+      <c r="EE9" s="124"/>
+      <c r="EF9" s="123"/>
+      <c r="EG9" s="124"/>
+      <c r="EH9" s="123"/>
+      <c r="EI9" s="132"/>
+      <c r="EJ9" s="132"/>
+      <c r="EK9" s="132"/>
+      <c r="EL9" s="132"/>
+      <c r="EM9" s="124"/>
+      <c r="EN9" s="123"/>
+      <c r="EO9" s="132"/>
+      <c r="EP9" s="124"/>
       <c r="EQ9" s="9"/>
       <c r="ER9" s="9"/>
       <c r="ES9" s="9"/>
@@ -13982,15 +15994,15 @@
       <c r="FH9" s="10"/>
     </row>
     <row r="10" spans="2:164">
-      <c r="F10" s="91" t="s">
+      <c r="F10" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="92"/>
-      <c r="L10" s="93"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="94"/>
+      <c r="I10" s="94"/>
+      <c r="J10" s="94"/>
+      <c r="K10" s="94"/>
+      <c r="L10" s="95"/>
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
@@ -14084,9 +16096,9 @@
       <c r="DJ10" s="9"/>
       <c r="DK10" s="19"/>
       <c r="DL10" s="9"/>
-      <c r="DM10" s="117"/>
-      <c r="DN10" s="118"/>
-      <c r="DO10" s="118"/>
+      <c r="DM10" s="119"/>
+      <c r="DN10" s="120"/>
+      <c r="DO10" s="120"/>
       <c r="DP10" s="18"/>
       <c r="DQ10" s="9"/>
       <c r="DR10" s="9"/>
@@ -14099,27 +16111,27 @@
       <c r="DY10" s="19"/>
       <c r="DZ10" s="10"/>
       <c r="EC10" s="8"/>
-      <c r="ED10" s="119" t="s">
+      <c r="ED10" s="121" t="s">
         <v>142</v>
       </c>
-      <c r="EE10" s="120"/>
-      <c r="EF10" s="132">
+      <c r="EE10" s="122"/>
+      <c r="EF10" s="134">
         <v>2</v>
       </c>
-      <c r="EG10" s="133"/>
-      <c r="EH10" s="123">
+      <c r="EG10" s="135"/>
+      <c r="EH10" s="125">
         <v>0</v>
       </c>
-      <c r="EI10" s="127"/>
-      <c r="EJ10" s="127"/>
-      <c r="EK10" s="127"/>
-      <c r="EL10" s="127"/>
-      <c r="EM10" s="124"/>
-      <c r="EN10" s="123">
+      <c r="EI10" s="129"/>
+      <c r="EJ10" s="129"/>
+      <c r="EK10" s="129"/>
+      <c r="EL10" s="129"/>
+      <c r="EM10" s="126"/>
+      <c r="EN10" s="125">
         <v>0</v>
       </c>
-      <c r="EO10" s="127"/>
-      <c r="EP10" s="124"/>
+      <c r="EO10" s="129"/>
+      <c r="EP10" s="126"/>
       <c r="EQ10" s="9"/>
       <c r="ER10" s="9"/>
       <c r="ES10" s="9"/>
@@ -14139,13 +16151,13 @@
       <c r="FH10" s="10"/>
     </row>
     <row r="11" spans="2:164" ht="17" thickBot="1">
-      <c r="F11" s="94"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="95"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="97"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="98"/>
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -14191,13 +16203,13 @@
       <c r="BH11" s="28"/>
       <c r="BI11" s="30"/>
       <c r="BJ11" s="9"/>
-      <c r="BK11" s="131" t="s">
+      <c r="BK11" s="133" t="s">
         <v>58</v>
       </c>
-      <c r="BL11" s="131"/>
-      <c r="BM11" s="131"/>
-      <c r="BN11" s="131"/>
-      <c r="BO11" s="131"/>
+      <c r="BL11" s="133"/>
+      <c r="BM11" s="133"/>
+      <c r="BN11" s="133"/>
+      <c r="BO11" s="133"/>
       <c r="BP11" s="9"/>
       <c r="BQ11" s="9"/>
       <c r="BR11" s="9"/>
@@ -14247,9 +16259,9 @@
       <c r="DJ11" s="9"/>
       <c r="DK11" s="19"/>
       <c r="DL11" s="9"/>
-      <c r="DM11" s="117"/>
-      <c r="DN11" s="118"/>
-      <c r="DO11" s="118"/>
+      <c r="DM11" s="119"/>
+      <c r="DN11" s="120"/>
+      <c r="DO11" s="120"/>
       <c r="DP11" s="18"/>
       <c r="DQ11" s="9"/>
       <c r="DR11" s="9"/>
@@ -14262,19 +16274,19 @@
       <c r="DY11" s="19"/>
       <c r="DZ11" s="10"/>
       <c r="EC11" s="8"/>
-      <c r="ED11" s="121"/>
-      <c r="EE11" s="122"/>
-      <c r="EF11" s="134"/>
-      <c r="EG11" s="135"/>
-      <c r="EH11" s="125"/>
-      <c r="EI11" s="128"/>
-      <c r="EJ11" s="128"/>
-      <c r="EK11" s="128"/>
-      <c r="EL11" s="128"/>
-      <c r="EM11" s="126"/>
-      <c r="EN11" s="125"/>
-      <c r="EO11" s="128"/>
-      <c r="EP11" s="126"/>
+      <c r="ED11" s="123"/>
+      <c r="EE11" s="124"/>
+      <c r="EF11" s="136"/>
+      <c r="EG11" s="137"/>
+      <c r="EH11" s="127"/>
+      <c r="EI11" s="130"/>
+      <c r="EJ11" s="130"/>
+      <c r="EK11" s="130"/>
+      <c r="EL11" s="130"/>
+      <c r="EM11" s="128"/>
+      <c r="EN11" s="127"/>
+      <c r="EO11" s="130"/>
+      <c r="EP11" s="128"/>
       <c r="EQ11" s="9"/>
       <c r="ER11" s="9"/>
       <c r="ES11" s="9"/>
@@ -14294,15 +16306,15 @@
       <c r="FH11" s="10"/>
     </row>
     <row r="12" spans="2:164" ht="16" customHeight="1">
-      <c r="F12" s="91" t="s">
+      <c r="F12" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="92"/>
-      <c r="L12" s="93"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="94"/>
+      <c r="I12" s="94"/>
+      <c r="J12" s="94"/>
+      <c r="K12" s="94"/>
+      <c r="L12" s="95"/>
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -14413,27 +16425,27 @@
       <c r="DY12" s="22"/>
       <c r="DZ12" s="10"/>
       <c r="EC12" s="8"/>
-      <c r="ED12" s="119" t="s">
+      <c r="ED12" s="121" t="s">
         <v>143</v>
       </c>
-      <c r="EE12" s="120"/>
-      <c r="EF12" s="132">
+      <c r="EE12" s="122"/>
+      <c r="EF12" s="134">
         <v>3</v>
       </c>
-      <c r="EG12" s="133"/>
-      <c r="EH12" s="123">
+      <c r="EG12" s="135"/>
+      <c r="EH12" s="125">
         <v>0</v>
       </c>
-      <c r="EI12" s="127"/>
-      <c r="EJ12" s="127"/>
-      <c r="EK12" s="127"/>
-      <c r="EL12" s="127"/>
-      <c r="EM12" s="124"/>
-      <c r="EN12" s="123">
+      <c r="EI12" s="129"/>
+      <c r="EJ12" s="129"/>
+      <c r="EK12" s="129"/>
+      <c r="EL12" s="129"/>
+      <c r="EM12" s="126"/>
+      <c r="EN12" s="125">
         <v>0</v>
       </c>
-      <c r="EO12" s="127"/>
-      <c r="EP12" s="124"/>
+      <c r="EO12" s="129"/>
+      <c r="EP12" s="126"/>
       <c r="EQ12" s="9"/>
       <c r="ER12" s="9"/>
       <c r="ES12" s="9"/>
@@ -14453,13 +16465,13 @@
       <c r="FH12" s="10"/>
     </row>
     <row r="13" spans="2:164" ht="17" thickBot="1">
-      <c r="F13" s="94"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="95"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="95"/>
-      <c r="K13" s="95"/>
-      <c r="L13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="98"/>
       <c r="M13" s="11"/>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
@@ -14578,19 +16590,19 @@
       <c r="DY13" s="22"/>
       <c r="DZ13" s="10"/>
       <c r="EC13" s="8"/>
-      <c r="ED13" s="121"/>
-      <c r="EE13" s="122"/>
-      <c r="EF13" s="134"/>
-      <c r="EG13" s="135"/>
-      <c r="EH13" s="125"/>
-      <c r="EI13" s="128"/>
-      <c r="EJ13" s="128"/>
-      <c r="EK13" s="128"/>
-      <c r="EL13" s="128"/>
-      <c r="EM13" s="126"/>
-      <c r="EN13" s="125"/>
-      <c r="EO13" s="128"/>
-      <c r="EP13" s="126"/>
+      <c r="ED13" s="123"/>
+      <c r="EE13" s="124"/>
+      <c r="EF13" s="136"/>
+      <c r="EG13" s="137"/>
+      <c r="EH13" s="127"/>
+      <c r="EI13" s="130"/>
+      <c r="EJ13" s="130"/>
+      <c r="EK13" s="130"/>
+      <c r="EL13" s="130"/>
+      <c r="EM13" s="128"/>
+      <c r="EN13" s="127"/>
+      <c r="EO13" s="130"/>
+      <c r="EP13" s="128"/>
       <c r="EQ13" s="9"/>
       <c r="ER13" s="9"/>
       <c r="ES13" s="9"/>
@@ -14610,15 +16622,15 @@
       <c r="FH13" s="10"/>
     </row>
     <row r="14" spans="2:164" ht="16" customHeight="1">
-      <c r="F14" s="91" t="s">
+      <c r="F14" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="93"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="94"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="95"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
@@ -14760,13 +16772,13 @@
       <c r="FH14" s="39"/>
     </row>
     <row r="15" spans="2:164" ht="17" thickBot="1">
-      <c r="F15" s="94"/>
-      <c r="G15" s="95"/>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="95"/>
-      <c r="L15" s="96"/>
+      <c r="F15" s="96"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="97"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="98"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
@@ -14918,15 +16930,15 @@
       <c r="FH15" s="10"/>
     </row>
     <row r="16" spans="2:164">
-      <c r="F16" s="91" t="s">
+      <c r="F16" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="92"/>
-      <c r="H16" s="92"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="92"/>
-      <c r="L16" s="93"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="95"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
@@ -15092,13 +17104,13 @@
       <c r="FH16" s="10"/>
     </row>
     <row r="17" spans="2:164" ht="17" customHeight="1" thickBot="1">
-      <c r="F17" s="94"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="97"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="98"/>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
@@ -15165,10 +17177,10 @@
       <c r="CG17" s="32"/>
       <c r="CH17" s="33"/>
       <c r="CK17" s="8"/>
-      <c r="CL17" s="115" t="s">
+      <c r="CL17" s="117" t="s">
         <v>107</v>
       </c>
-      <c r="CM17" s="116"/>
+      <c r="CM17" s="118"/>
       <c r="CN17" s="9"/>
       <c r="CO17" s="28"/>
       <c r="CP17" s="29"/>
@@ -15237,42 +17249,42 @@
       <c r="ES17" s="30">
         <v>1</v>
       </c>
-      <c r="ET17" s="136">
+      <c r="ET17" s="138">
         <v>10</v>
       </c>
-      <c r="EU17" s="137"/>
-      <c r="EV17" s="136">
+      <c r="EU17" s="139"/>
+      <c r="EV17" s="138">
         <v>5</v>
       </c>
-      <c r="EW17" s="137"/>
+      <c r="EW17" s="139"/>
       <c r="EX17" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="EY17" s="136">
+      <c r="EY17" s="138">
         <v>0</v>
       </c>
-      <c r="EZ17" s="138"/>
-      <c r="FA17" s="137"/>
-      <c r="FB17" s="139"/>
-      <c r="FC17" s="140"/>
-      <c r="FD17" s="139"/>
-      <c r="FE17" s="140"/>
-      <c r="FF17" s="139" t="s">
+      <c r="EZ17" s="140"/>
+      <c r="FA17" s="139"/>
+      <c r="FB17" s="141"/>
+      <c r="FC17" s="142"/>
+      <c r="FD17" s="141"/>
+      <c r="FE17" s="142"/>
+      <c r="FF17" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="FG17" s="141"/>
+      <c r="FG17" s="143"/>
       <c r="FH17" s="10"/>
     </row>
     <row r="18" spans="2:164" ht="16" customHeight="1">
-      <c r="F18" s="91" t="s">
+      <c r="F18" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="92"/>
-      <c r="H18" s="92"/>
-      <c r="I18" s="92"/>
-      <c r="J18" s="92"/>
-      <c r="K18" s="92"/>
-      <c r="L18" s="93"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="95"/>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
@@ -15341,8 +17353,8 @@
       <c r="CG18" s="9"/>
       <c r="CH18" s="10"/>
       <c r="CK18" s="8"/>
-      <c r="CL18" s="115"/>
-      <c r="CM18" s="116"/>
+      <c r="CL18" s="117"/>
+      <c r="CM18" s="118"/>
       <c r="CN18" s="9"/>
       <c r="CO18" s="9"/>
       <c r="CP18" s="9"/>
@@ -15411,40 +17423,40 @@
       <c r="ES18" s="30">
         <v>1</v>
       </c>
-      <c r="ET18" s="136">
+      <c r="ET18" s="138">
         <v>11</v>
       </c>
-      <c r="EU18" s="137"/>
-      <c r="EV18" s="136">
+      <c r="EU18" s="139"/>
+      <c r="EV18" s="138">
         <v>6</v>
       </c>
-      <c r="EW18" s="137"/>
+      <c r="EW18" s="139"/>
       <c r="EX18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="EY18" s="136">
+      <c r="EY18" s="138">
         <v>1</v>
       </c>
-      <c r="EZ18" s="138"/>
-      <c r="FA18" s="137"/>
-      <c r="FB18" s="139"/>
-      <c r="FC18" s="140"/>
-      <c r="FD18" s="139"/>
-      <c r="FE18" s="140"/>
-      <c r="FF18" s="139" t="s">
+      <c r="EZ18" s="140"/>
+      <c r="FA18" s="139"/>
+      <c r="FB18" s="141"/>
+      <c r="FC18" s="142"/>
+      <c r="FD18" s="141"/>
+      <c r="FE18" s="142"/>
+      <c r="FF18" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="FG18" s="141"/>
+      <c r="FG18" s="143"/>
       <c r="FH18" s="10"/>
     </row>
     <row r="19" spans="2:164" ht="17" customHeight="1" thickBot="1">
-      <c r="F19" s="94"/>
-      <c r="G19" s="95"/>
-      <c r="H19" s="95"/>
-      <c r="I19" s="95"/>
-      <c r="J19" s="95"/>
-      <c r="K19" s="95"/>
-      <c r="L19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="97"/>
+      <c r="K19" s="97"/>
+      <c r="L19" s="98"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
@@ -15511,8 +17523,8 @@
       <c r="CG19" s="9"/>
       <c r="CH19" s="10"/>
       <c r="CK19" s="8"/>
-      <c r="CL19" s="115"/>
-      <c r="CM19" s="116"/>
+      <c r="CL19" s="117"/>
+      <c r="CM19" s="118"/>
       <c r="CN19" s="9"/>
       <c r="CO19" s="9"/>
       <c r="CP19" s="9"/>
@@ -15581,42 +17593,42 @@
       <c r="ES19" s="30">
         <v>1</v>
       </c>
-      <c r="ET19" s="136">
+      <c r="ET19" s="138">
         <v>12</v>
       </c>
-      <c r="EU19" s="137"/>
-      <c r="EV19" s="136">
+      <c r="EU19" s="139"/>
+      <c r="EV19" s="138">
         <v>7</v>
       </c>
-      <c r="EW19" s="137"/>
+      <c r="EW19" s="139"/>
       <c r="EX19" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="EY19" s="136">
+      <c r="EY19" s="138">
         <v>2</v>
       </c>
-      <c r="EZ19" s="138"/>
-      <c r="FA19" s="137"/>
-      <c r="FB19" s="139"/>
-      <c r="FC19" s="140"/>
-      <c r="FD19" s="139"/>
-      <c r="FE19" s="140"/>
-      <c r="FF19" s="139" t="s">
+      <c r="EZ19" s="140"/>
+      <c r="FA19" s="139"/>
+      <c r="FB19" s="141"/>
+      <c r="FC19" s="142"/>
+      <c r="FD19" s="141"/>
+      <c r="FE19" s="142"/>
+      <c r="FF19" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="FG19" s="141"/>
+      <c r="FG19" s="143"/>
       <c r="FH19" s="10"/>
     </row>
     <row r="20" spans="2:164" ht="16" customHeight="1">
-      <c r="F20" s="91" t="s">
+      <c r="F20" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="92"/>
-      <c r="H20" s="92"/>
-      <c r="I20" s="92"/>
-      <c r="J20" s="92"/>
-      <c r="K20" s="92"/>
-      <c r="L20" s="93"/>
+      <c r="G20" s="94"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="94"/>
+      <c r="J20" s="94"/>
+      <c r="K20" s="94"/>
+      <c r="L20" s="95"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
@@ -15640,32 +17652,32 @@
       <c r="AG20" s="9"/>
       <c r="AH20" s="10"/>
       <c r="AR20" s="8"/>
-      <c r="AS20" s="119" t="s">
+      <c r="AS20" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="AT20" s="120"/>
-      <c r="AU20" s="119" t="s">
+      <c r="AT20" s="122"/>
+      <c r="AU20" s="121" t="s">
         <v>70</v>
       </c>
-      <c r="AV20" s="120"/>
-      <c r="AW20" s="119" t="s">
+      <c r="AV20" s="122"/>
+      <c r="AW20" s="121" t="s">
         <v>71</v>
       </c>
-      <c r="AX20" s="129"/>
-      <c r="AY20" s="129"/>
-      <c r="AZ20" s="129"/>
-      <c r="BA20" s="129"/>
-      <c r="BB20" s="120"/>
-      <c r="BC20" s="119" t="s">
+      <c r="AX20" s="131"/>
+      <c r="AY20" s="131"/>
+      <c r="AZ20" s="131"/>
+      <c r="BA20" s="131"/>
+      <c r="BB20" s="122"/>
+      <c r="BC20" s="121" t="s">
         <v>72</v>
       </c>
-      <c r="BD20" s="129"/>
-      <c r="BE20" s="120"/>
-      <c r="BF20" s="119" t="s">
+      <c r="BD20" s="131"/>
+      <c r="BE20" s="122"/>
+      <c r="BF20" s="121" t="s">
         <v>74</v>
       </c>
-      <c r="BG20" s="129"/>
-      <c r="BH20" s="120"/>
+      <c r="BG20" s="131"/>
+      <c r="BH20" s="122"/>
       <c r="BI20" s="9"/>
       <c r="BJ20" s="9" t="s">
         <v>76</v>
@@ -15771,40 +17783,40 @@
       <c r="ES20" s="30">
         <v>1</v>
       </c>
-      <c r="ET20" s="136">
+      <c r="ET20" s="138">
         <v>13</v>
       </c>
-      <c r="EU20" s="137"/>
-      <c r="EV20" s="136">
+      <c r="EU20" s="139"/>
+      <c r="EV20" s="138">
         <v>8</v>
       </c>
-      <c r="EW20" s="137"/>
+      <c r="EW20" s="139"/>
       <c r="EX20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="EY20" s="136">
+      <c r="EY20" s="138">
         <v>3</v>
       </c>
-      <c r="EZ20" s="138"/>
-      <c r="FA20" s="137"/>
-      <c r="FB20" s="139"/>
-      <c r="FC20" s="140"/>
-      <c r="FD20" s="139"/>
-      <c r="FE20" s="140"/>
-      <c r="FF20" s="139" t="s">
+      <c r="EZ20" s="140"/>
+      <c r="FA20" s="139"/>
+      <c r="FB20" s="141"/>
+      <c r="FC20" s="142"/>
+      <c r="FD20" s="141"/>
+      <c r="FE20" s="142"/>
+      <c r="FF20" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="FG20" s="141"/>
+      <c r="FG20" s="143"/>
       <c r="FH20" s="10"/>
     </row>
     <row r="21" spans="2:164" ht="17" customHeight="1" thickBot="1">
-      <c r="F21" s="94"/>
-      <c r="G21" s="95"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="95"/>
-      <c r="J21" s="95"/>
-      <c r="K21" s="95"/>
-      <c r="L21" s="96"/>
+      <c r="F21" s="96"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="97"/>
+      <c r="I21" s="97"/>
+      <c r="J21" s="97"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="98"/>
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
@@ -15828,22 +17840,22 @@
       <c r="AG21" s="12"/>
       <c r="AH21" s="13"/>
       <c r="AR21" s="8"/>
-      <c r="AS21" s="121"/>
-      <c r="AT21" s="122"/>
-      <c r="AU21" s="121"/>
-      <c r="AV21" s="122"/>
-      <c r="AW21" s="121"/>
-      <c r="AX21" s="130"/>
-      <c r="AY21" s="130"/>
-      <c r="AZ21" s="130"/>
-      <c r="BA21" s="130"/>
-      <c r="BB21" s="122"/>
-      <c r="BC21" s="121"/>
-      <c r="BD21" s="130"/>
-      <c r="BE21" s="122"/>
-      <c r="BF21" s="121"/>
-      <c r="BG21" s="130"/>
-      <c r="BH21" s="122"/>
+      <c r="AS21" s="123"/>
+      <c r="AT21" s="124"/>
+      <c r="AU21" s="123"/>
+      <c r="AV21" s="124"/>
+      <c r="AW21" s="123"/>
+      <c r="AX21" s="132"/>
+      <c r="AY21" s="132"/>
+      <c r="AZ21" s="132"/>
+      <c r="BA21" s="132"/>
+      <c r="BB21" s="124"/>
+      <c r="BC21" s="123"/>
+      <c r="BD21" s="132"/>
+      <c r="BE21" s="124"/>
+      <c r="BF21" s="123"/>
+      <c r="BG21" s="132"/>
+      <c r="BH21" s="124"/>
       <c r="BI21" s="9"/>
       <c r="BJ21" s="9"/>
       <c r="BK21" s="9"/>
@@ -15945,30 +17957,30 @@
       <c r="ES21" s="30">
         <v>1</v>
       </c>
-      <c r="ET21" s="136">
+      <c r="ET21" s="138">
         <v>14</v>
       </c>
-      <c r="EU21" s="137"/>
-      <c r="EV21" s="136">
+      <c r="EU21" s="139"/>
+      <c r="EV21" s="138">
         <v>9</v>
       </c>
-      <c r="EW21" s="137"/>
+      <c r="EW21" s="139"/>
       <c r="EX21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="EY21" s="136">
+      <c r="EY21" s="138">
         <v>4</v>
       </c>
-      <c r="EZ21" s="138"/>
-      <c r="FA21" s="137"/>
-      <c r="FB21" s="139"/>
-      <c r="FC21" s="140"/>
-      <c r="FD21" s="139"/>
-      <c r="FE21" s="140"/>
-      <c r="FF21" s="139" t="s">
+      <c r="EZ21" s="140"/>
+      <c r="FA21" s="139"/>
+      <c r="FB21" s="141"/>
+      <c r="FC21" s="142"/>
+      <c r="FD21" s="141"/>
+      <c r="FE21" s="142"/>
+      <c r="FF21" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="FG21" s="141"/>
+      <c r="FG21" s="143"/>
       <c r="FH21" s="10"/>
     </row>
     <row r="22" spans="2:164">
@@ -16002,32 +18014,32 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="7"/>
       <c r="AR22" s="8"/>
-      <c r="AS22" s="119" t="s">
+      <c r="AS22" s="121" t="s">
         <v>73</v>
       </c>
-      <c r="AT22" s="120"/>
-      <c r="AU22" s="123">
+      <c r="AT22" s="122"/>
+      <c r="AU22" s="125">
         <v>30</v>
       </c>
-      <c r="AV22" s="124"/>
-      <c r="AW22" s="123">
+      <c r="AV22" s="126"/>
+      <c r="AW22" s="125">
         <v>0</v>
       </c>
-      <c r="AX22" s="127"/>
-      <c r="AY22" s="127"/>
-      <c r="AZ22" s="127"/>
-      <c r="BA22" s="127"/>
-      <c r="BB22" s="124"/>
-      <c r="BC22" s="123">
+      <c r="AX22" s="129"/>
+      <c r="AY22" s="129"/>
+      <c r="AZ22" s="129"/>
+      <c r="BA22" s="129"/>
+      <c r="BB22" s="126"/>
+      <c r="BC22" s="125">
         <v>0</v>
       </c>
-      <c r="BD22" s="127"/>
-      <c r="BE22" s="124"/>
-      <c r="BF22" s="119" t="s">
+      <c r="BD22" s="129"/>
+      <c r="BE22" s="126"/>
+      <c r="BF22" s="121" t="s">
         <v>75</v>
       </c>
-      <c r="BG22" s="129"/>
-      <c r="BH22" s="120"/>
+      <c r="BG22" s="131"/>
+      <c r="BH22" s="122"/>
       <c r="BI22" s="9"/>
       <c r="BJ22" s="9"/>
       <c r="BK22" s="9"/>
@@ -16165,22 +18177,22 @@
         <v>35</v>
       </c>
       <c r="AR23" s="8"/>
-      <c r="AS23" s="121"/>
-      <c r="AT23" s="122"/>
-      <c r="AU23" s="125"/>
-      <c r="AV23" s="126"/>
-      <c r="AW23" s="125"/>
-      <c r="AX23" s="128"/>
-      <c r="AY23" s="128"/>
-      <c r="AZ23" s="128"/>
-      <c r="BA23" s="128"/>
-      <c r="BB23" s="126"/>
-      <c r="BC23" s="125"/>
-      <c r="BD23" s="128"/>
-      <c r="BE23" s="126"/>
-      <c r="BF23" s="121"/>
-      <c r="BG23" s="130"/>
-      <c r="BH23" s="122"/>
+      <c r="AS23" s="123"/>
+      <c r="AT23" s="124"/>
+      <c r="AU23" s="127"/>
+      <c r="AV23" s="128"/>
+      <c r="AW23" s="127"/>
+      <c r="AX23" s="130"/>
+      <c r="AY23" s="130"/>
+      <c r="AZ23" s="130"/>
+      <c r="BA23" s="130"/>
+      <c r="BB23" s="128"/>
+      <c r="BC23" s="127"/>
+      <c r="BD23" s="130"/>
+      <c r="BE23" s="128"/>
+      <c r="BF23" s="123"/>
+      <c r="BG23" s="132"/>
+      <c r="BH23" s="124"/>
       <c r="BI23" s="9"/>
       <c r="BJ23" s="9"/>
       <c r="BK23" s="9"/>
@@ -17486,10 +19498,10 @@
       <c r="CG36" s="9"/>
       <c r="CH36" s="10"/>
       <c r="CK36" s="8"/>
-      <c r="CL36" s="115" t="s">
+      <c r="CL36" s="117" t="s">
         <v>107</v>
       </c>
-      <c r="CM36" s="116"/>
+      <c r="CM36" s="118"/>
       <c r="CN36" s="9"/>
       <c r="CO36" s="28"/>
       <c r="CP36" s="29"/>
@@ -17575,8 +19587,8 @@
       <c r="CG37" s="9"/>
       <c r="CH37" s="10"/>
       <c r="CK37" s="8"/>
-      <c r="CL37" s="115"/>
-      <c r="CM37" s="116"/>
+      <c r="CL37" s="117"/>
+      <c r="CM37" s="118"/>
       <c r="CN37" s="9"/>
       <c r="CO37" s="9"/>
       <c r="CP37" s="9"/>
@@ -17663,8 +19675,8 @@
       <c r="CG38" s="38"/>
       <c r="CH38" s="39"/>
       <c r="CK38" s="8"/>
-      <c r="CL38" s="115"/>
-      <c r="CM38" s="116"/>
+      <c r="CL38" s="117"/>
+      <c r="CM38" s="118"/>
       <c r="CN38" s="9"/>
       <c r="CO38" s="9"/>
       <c r="CP38" s="9"/>
@@ -18705,7 +20717,7 @@
   <dimension ref="B2:AY33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AI11" sqref="AI11"/>
+      <selection activeCell="AO13" sqref="AO13:AX13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="16"/>
@@ -19420,12 +21432,12 @@
       <c r="AR15" s="16"/>
       <c r="AS15" s="16"/>
       <c r="AT15" s="16"/>
-      <c r="AU15" s="119" t="s">
+      <c r="AU15" s="121" t="s">
         <v>74</v>
       </c>
-      <c r="AV15" s="129"/>
-      <c r="AW15" s="129"/>
-      <c r="AX15" s="120"/>
+      <c r="AV15" s="131"/>
+      <c r="AW15" s="131"/>
+      <c r="AX15" s="122"/>
       <c r="AY15" s="10"/>
     </row>
     <row r="16" spans="2:51">
@@ -19472,10 +21484,10 @@
       <c r="AR16" s="21"/>
       <c r="AS16" s="21"/>
       <c r="AT16" s="21"/>
-      <c r="AU16" s="121"/>
-      <c r="AV16" s="130"/>
-      <c r="AW16" s="130"/>
-      <c r="AX16" s="122"/>
+      <c r="AU16" s="123"/>
+      <c r="AV16" s="132"/>
+      <c r="AW16" s="132"/>
+      <c r="AX16" s="124"/>
       <c r="AY16" s="10"/>
     </row>
     <row r="17" spans="4:51">

</xml_diff>

<commit_message>
Update Container Booking Registration
</commit_message>
<xml_diff>
--- a/Specification/General Design Specification - Transport Management System.xlsx
+++ b/Specification/General Design Specification - Transport Management System.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/Personal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5F4CB4-F3C3-AF4B-97BA-466787400DC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BEFC9D-0ACA-DC4F-A120-F19C5E51B936}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14440" firstSheet="6" activeTab="9" xr2:uid="{E7A8EFBF-D4F9-BE40-861A-BF0B4B9B5190}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14440" firstSheet="7" activeTab="10" xr2:uid="{E7A8EFBF-D4F9-BE40-861A-BF0B4B9B5190}"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="250">
   <si>
     <t>No.</t>
   </si>
@@ -900,6 +900,9 @@
   </si>
   <si>
     <t>Khi click vao search button thi show thong tin mau xam tu thong tin booking da tao.</t>
+  </si>
+  <si>
+    <t>DRV0003</t>
   </si>
 </sst>
 </file>
@@ -6260,7 +6263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E1F607D-F349-1E4C-A80B-CC18273F07C4}">
   <dimension ref="B2:AM29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="AP19" sqref="AP19"/>
     </sheetView>
   </sheetViews>
@@ -7262,8 +7265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{074DFE09-608C-C946-A127-D7CE93149F2F}">
   <dimension ref="C2:AV76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:AQ18"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="AD54" sqref="AD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
@@ -10204,7 +10207,7 @@
       <c r="AE62" s="73"/>
       <c r="AF62" s="72"/>
       <c r="AG62" s="83" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="AH62" s="84"/>
       <c r="AI62" s="89" t="s">
@@ -10324,7 +10327,7 @@
       <c r="AE64" s="73"/>
       <c r="AF64" s="72"/>
       <c r="AG64" s="83" t="s">
-        <v>206</v>
+        <v>249</v>
       </c>
       <c r="AH64" s="84"/>
       <c r="AI64" s="89" t="s">
@@ -10566,7 +10569,7 @@
   <dimension ref="B1:AV33"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="AR27" sqref="AR27"/>
+      <selection activeCell="AH31" sqref="AH31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="16"/>
@@ -20717,7 +20720,7 @@
   <dimension ref="B2:AY33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AO13" sqref="AO13:AX13"/>
+      <selection activeCell="AE25" sqref="AE25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="16"/>

</xml_diff>